<commit_message>
Add data for 2021-09-30
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-22" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -734,13 +734,13 @@
         <v>0.06759999999999999</v>
       </c>
       <c r="T3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U3" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0.0648</v>
+        <v>0.0694</v>
       </c>
     </row>
     <row r="4">
@@ -1230,7 +1230,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-21)</t>
+          <t>September (through 09-22)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1255,40 +1255,40 @@
         <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.08160000000000001</v>
+        <v>0.0784</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.075</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="N11" t="n">
         <v>4</v>
       </c>
       <c r="O11" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0727</v>
       </c>
       <c r="Q11" t="n">
         <v>3</v>
       </c>
       <c r="R11" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0366</v>
+        <v>0.0357</v>
       </c>
       <c r="U11" t="n">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12">
@@ -1319,46 +1319,46 @@
         <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.08169999999999999</v>
+        <v>0.0814</v>
       </c>
       <c r="K12" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.1147</v>
       </c>
       <c r="N12" t="n">
         <v>40</v>
       </c>
       <c r="O12" t="n">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1003</v>
+        <v>0.099</v>
       </c>
       <c r="Q12" t="n">
         <v>51</v>
       </c>
       <c r="R12" t="n">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0589</v>
+        <v>0.0588</v>
       </c>
       <c r="T12" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U12" t="n">
-        <v>1125</v>
+        <v>1130</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0602</v>
+        <v>0.0607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-01
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-23" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1221,26 +1221,26 @@
         <v>5</v>
       </c>
       <c r="U10" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0316</v>
+        <v>0.0314</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-22)</t>
+          <t>September (through 09-23)</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.0435</v>
+        <v>0.04</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
@@ -1255,40 +1255,40 @@
         <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0784</v>
+        <v>0.0702</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O11" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.0727</v>
+        <v>0.0877</v>
       </c>
       <c r="Q11" t="n">
         <v>3</v>
       </c>
       <c r="R11" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0357</v>
+        <v>0.0345</v>
       </c>
       <c r="U11" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12">
@@ -1301,10 +1301,10 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1382</v>
+        <v>0.137</v>
       </c>
       <c r="E12" t="n">
         <v>43</v>
@@ -1319,46 +1319,46 @@
         <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0814</v>
+        <v>0.0806</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1147</v>
+        <v>0.1138</v>
       </c>
       <c r="N12" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O12" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.099</v>
+        <v>0.101</v>
       </c>
       <c r="Q12" t="n">
         <v>51</v>
       </c>
       <c r="R12" t="n">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0586</v>
       </c>
       <c r="T12" t="n">
         <v>73</v>
       </c>
       <c r="U12" t="n">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0607</v>
+        <v>0.0605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-02
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-23" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-24" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1151,10 +1151,10 @@
         <v>10</v>
       </c>
       <c r="U9" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.0658</v>
+        <v>0.06619999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1218,19 +1218,19 @@
         <v>0.0491</v>
       </c>
       <c r="T10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U10" t="n">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0314</v>
+        <v>0.0377</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-23)</t>
+          <t>September (through 09-24)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1246,49 +1246,55 @@
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0571</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0702</v>
+        <v>0.0667</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.0851</v>
       </c>
       <c r="N11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.1</v>
       </c>
       <c r="Q11" t="n">
         <v>3</v>
       </c>
       <c r="R11" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0345</v>
+        <v>0.0323</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1</v>
       </c>
       <c r="U11" t="n">
-        <v>135</v>
+        <v>141</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>0.007</v>
       </c>
     </row>
     <row r="12">
@@ -1310,55 +1316,55 @@
         <v>43</v>
       </c>
       <c r="F12" t="n">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1036</v>
+        <v>0.1034</v>
       </c>
       <c r="H12" t="n">
         <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1138</v>
+        <v>0.1136</v>
       </c>
       <c r="N12" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O12" t="n">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.101</v>
+        <v>0.1027</v>
       </c>
       <c r="Q12" t="n">
         <v>51</v>
       </c>
       <c r="R12" t="n">
-        <v>820</v>
+        <v>826</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0586</v>
+        <v>0.0582</v>
       </c>
       <c r="T12" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="U12" t="n">
-        <v>1133</v>
+        <v>1137</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0605</v>
+        <v>0.0619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-03
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-25" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -929,13 +929,13 @@
         <v>0.08890000000000001</v>
       </c>
       <c r="Q6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R6" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.0469</v>
       </c>
       <c r="T6" t="n">
         <v>10</v>
@@ -1230,7 +1230,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-24)</t>
+          <t>September (through 09-25)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1246,55 +1246,55 @@
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.0571</v>
+        <v>0.0556</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.0625</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.0851</v>
+        <v>0.08160000000000001</v>
       </c>
       <c r="N11" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0984</v>
       </c>
       <c r="Q11" t="n">
         <v>3</v>
       </c>
       <c r="R11" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0323</v>
+        <v>0.0306</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.007</v>
+        <v>0.0132</v>
       </c>
     </row>
     <row r="12">
@@ -1316,55 +1316,55 @@
         <v>43</v>
       </c>
       <c r="F12" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1031</v>
       </c>
       <c r="H12" t="n">
         <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1136</v>
+        <v>0.1132</v>
       </c>
       <c r="N12" t="n">
         <v>42</v>
       </c>
       <c r="O12" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1027</v>
+        <v>0.1024</v>
       </c>
       <c r="Q12" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R12" t="n">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0582</v>
+        <v>0.0567</v>
       </c>
       <c r="T12" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U12" t="n">
-        <v>1137</v>
+        <v>1146</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0619</v>
+        <v>0.0622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-04
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-25" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-26" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1230,71 +1230,71 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-25)</t>
+          <t>September (through 09-26)</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.04</v>
+        <v>0.037</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.0556</v>
+        <v>0.0769</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.0746</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.08160000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="N11" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.0984</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="Q11" t="n">
         <v>3</v>
       </c>
       <c r="R11" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0306</v>
+        <v>0.0303</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0132</v>
+        <v>0.0122</v>
       </c>
     </row>
     <row r="12">
@@ -1307,64 +1307,64 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.137</v>
+        <v>0.1357</v>
       </c>
       <c r="E12" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" t="n">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1048</v>
       </c>
       <c r="H12" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I12" t="n">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.07969999999999999</v>
+        <v>0.0809</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.113</v>
       </c>
       <c r="N12" t="n">
         <v>42</v>
       </c>
       <c r="O12" t="n">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1024</v>
+        <v>0.1019</v>
       </c>
       <c r="Q12" t="n">
         <v>50</v>
       </c>
       <c r="R12" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0567</v>
+        <v>0.0566</v>
       </c>
       <c r="T12" t="n">
         <v>76</v>
       </c>
       <c r="U12" t="n">
-        <v>1146</v>
+        <v>1158</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0622</v>
+        <v>0.0616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-05
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-26" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-27" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -929,13 +929,13 @@
         <v>0.08890000000000001</v>
       </c>
       <c r="Q6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>0.0469</v>
+        <v>0.0625</v>
       </c>
       <c r="T6" t="n">
         <v>10</v>
@@ -1230,35 +1230,35 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-26)</t>
+          <t>September (through 09-27)</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.037</v>
+        <v>0.0357</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.09760000000000001</v>
       </c>
       <c r="H11" t="n">
         <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0746</v>
+        <v>0.0725</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
@@ -1273,28 +1273,28 @@
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.09229999999999999</v>
       </c>
       <c r="Q11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0303</v>
+        <v>0.0388</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0122</v>
+        <v>0.0121</v>
       </c>
     </row>
     <row r="12">
@@ -1307,28 +1307,28 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1357</v>
+        <v>0.1351</v>
       </c>
       <c r="E12" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12" t="n">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1066</v>
       </c>
       <c r="H12" t="n">
         <v>50</v>
       </c>
       <c r="I12" t="n">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0809</v>
+        <v>0.0806</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
@@ -1343,28 +1343,28 @@
         <v>42</v>
       </c>
       <c r="O12" t="n">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1019</v>
+        <v>0.1014</v>
       </c>
       <c r="Q12" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R12" t="n">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0566</v>
+        <v>0.0586</v>
       </c>
       <c r="T12" t="n">
         <v>76</v>
       </c>
       <c r="U12" t="n">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0616</v>
+        <v>0.0615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-06
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-27" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-28" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1218,19 +1218,19 @@
         <v>0.0491</v>
       </c>
       <c r="T10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U10" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0377</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-27)</t>
+          <t>September (through 09-28)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1246,55 +1246,55 @@
         <v>4</v>
       </c>
       <c r="F11" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.09760000000000001</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="H11" t="n">
         <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0725</v>
+        <v>0.0694</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0769</v>
       </c>
       <c r="N11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O11" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.09229999999999999</v>
+        <v>0.1029</v>
       </c>
       <c r="Q11" t="n">
         <v>4</v>
       </c>
       <c r="R11" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0388</v>
+        <v>0.0374</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0121</v>
+        <v>0.0119</v>
       </c>
     </row>
     <row r="12">
@@ -1316,55 +1316,55 @@
         <v>45</v>
       </c>
       <c r="F12" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1066</v>
+        <v>0.1064</v>
       </c>
       <c r="H12" t="n">
         <v>50</v>
       </c>
       <c r="I12" t="n">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.0803</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.113</v>
+        <v>0.1125</v>
       </c>
       <c r="N12" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O12" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1014</v>
+        <v>0.1031</v>
       </c>
       <c r="Q12" t="n">
         <v>52</v>
       </c>
       <c r="R12" t="n">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0586</v>
+        <v>0.0584</v>
       </c>
       <c r="T12" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U12" t="n">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0615</v>
+        <v>0.0622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-07
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-28" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-29" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1148,13 +1148,13 @@
         <v>0.0201</v>
       </c>
       <c r="T9" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U9" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.06619999999999999</v>
+        <v>0.0728</v>
       </c>
     </row>
     <row r="10">
@@ -1230,71 +1230,71 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-28)</t>
+          <t>September (through 09-29)</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.0357</v>
+        <v>0.0333</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.1136</v>
       </c>
       <c r="H11" t="n">
         <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0694</v>
+        <v>0.06759999999999999</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.0741</v>
       </c>
       <c r="N11" t="n">
         <v>7</v>
       </c>
       <c r="O11" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.1029</v>
+        <v>0.09859999999999999</v>
       </c>
       <c r="Q11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R11" t="n">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0374</v>
+        <v>0.0446</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0119</v>
+        <v>0.0116</v>
       </c>
     </row>
     <row r="12">
@@ -1307,64 +1307,64 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1351</v>
+        <v>0.1339</v>
       </c>
       <c r="E12" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F12" t="n">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1064</v>
+        <v>0.1082</v>
       </c>
       <c r="H12" t="n">
         <v>50</v>
       </c>
       <c r="I12" t="n">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0803</v>
+        <v>0.08</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1125</v>
+        <v>0.1121</v>
       </c>
       <c r="N12" t="n">
         <v>43</v>
       </c>
       <c r="O12" t="n">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1024</v>
       </c>
       <c r="Q12" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R12" t="n">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0584</v>
+        <v>0.0592</v>
       </c>
       <c r="T12" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U12" t="n">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0622</v>
+        <v>0.06279999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-08
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-29" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-09-30" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1230,71 +1230,71 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-29)</t>
+          <t>September (through 09-30)</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.0333</v>
+        <v>0.0312</v>
       </c>
       <c r="E11" t="n">
         <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.1136</v>
+        <v>0.1042</v>
       </c>
       <c r="H11" t="n">
         <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.06759999999999999</v>
+        <v>0.0658</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
       </c>
       <c r="L11" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.0741</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="N11" t="n">
         <v>7</v>
       </c>
       <c r="O11" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.09859999999999999</v>
+        <v>0.0959</v>
       </c>
       <c r="Q11" t="n">
         <v>5</v>
       </c>
       <c r="R11" t="n">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>0.0446</v>
+        <v>0.0427</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="n">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0116</v>
+        <v>0.0112</v>
       </c>
     </row>
     <row r="12">
@@ -1307,64 +1307,64 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1339</v>
+        <v>0.1327</v>
       </c>
       <c r="E12" t="n">
         <v>46</v>
       </c>
       <c r="F12" t="n">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1082</v>
+        <v>0.1072</v>
       </c>
       <c r="H12" t="n">
         <v>50</v>
       </c>
       <c r="I12" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.08</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="K12" t="n">
         <v>61</v>
       </c>
       <c r="L12" t="n">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.1121</v>
+        <v>0.1113</v>
       </c>
       <c r="N12" t="n">
         <v>43</v>
       </c>
       <c r="O12" t="n">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1024</v>
+        <v>0.1019</v>
       </c>
       <c r="Q12" t="n">
         <v>53</v>
       </c>
       <c r="R12" t="n">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0592</v>
+        <v>0.0588</v>
       </c>
       <c r="T12" t="n">
         <v>78</v>
       </c>
       <c r="U12" t="n">
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.06279999999999999</v>
+        <v>0.0625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-09
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-30" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-01" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25.7109375" customWidth="1" min="1" max="1"/>
+    <col width="23.7109375" customWidth="1" min="1" max="1"/>
     <col width="11.7109375" customWidth="1" min="2" max="2"/>
     <col width="14.7109375" customWidth="1" min="3" max="3"/>
     <col width="11.7109375" customWidth="1" style="1" min="4" max="4"/>
@@ -1230,7 +1230,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>September (through 09-30)</t>
+          <t>September</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1300,71 +1300,99 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
+          <t>October (through 10-01)</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>0.1667</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4</v>
+      </c>
+      <c r="U12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>30</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>196</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.1327</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E13" t="n">
         <v>46</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F13" t="n">
         <v>383</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G13" s="1" t="n">
         <v>0.1072</v>
       </c>
-      <c r="H12" t="n">
-        <v>50</v>
-      </c>
-      <c r="I12" t="n">
-        <v>577</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>0.07969999999999999</v>
-      </c>
-      <c r="K12" t="n">
+      <c r="H13" t="n">
+        <v>51</v>
+      </c>
+      <c r="I13" t="n">
+        <v>582</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>0.0806</v>
+      </c>
+      <c r="K13" t="n">
         <v>61</v>
       </c>
-      <c r="L12" t="n">
-        <v>487</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>0.1113</v>
-      </c>
-      <c r="N12" t="n">
+      <c r="L13" t="n">
+        <v>490</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.1107</v>
+      </c>
+      <c r="N13" t="n">
         <v>43</v>
       </c>
-      <c r="O12" t="n">
-        <v>379</v>
-      </c>
-      <c r="P12" s="1" t="n">
-        <v>0.1019</v>
-      </c>
-      <c r="Q12" t="n">
+      <c r="O13" t="n">
+        <v>380</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>0.1017</v>
+      </c>
+      <c r="Q13" t="n">
         <v>53</v>
       </c>
-      <c r="R12" t="n">
-        <v>848</v>
-      </c>
-      <c r="S12" s="1" t="n">
-        <v>0.0588</v>
-      </c>
-      <c r="T12" t="n">
+      <c r="R13" t="n">
+        <v>852</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>0.0586</v>
+      </c>
+      <c r="T13" t="n">
         <v>78</v>
       </c>
-      <c r="U12" t="n">
-        <v>1170</v>
-      </c>
-      <c r="V12" s="1" t="n">
-        <v>0.0625</v>
+      <c r="U13" t="n">
+        <v>1178</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>0.0621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-10
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-02" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,29 +1300,35 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-01)</t>
-        </is>
+          <t>October (through 10-02)</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
+        <v>6</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L12" t="n">
         <v>5</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>0.1667</v>
-      </c>
-      <c r="L12" t="n">
-        <v>3</v>
       </c>
       <c r="O12" t="n">
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="U12" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -1335,37 +1341,37 @@
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1327</v>
+        <v>0.131</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1072</v>
+        <v>0.1057</v>
       </c>
       <c r="H13" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I13" t="n">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.0819</v>
       </c>
       <c r="K13" t="n">
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1107</v>
+        <v>0.1103</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
@@ -1380,19 +1386,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0586</v>
+        <v>0.0582</v>
       </c>
       <c r="T13" t="n">
         <v>78</v>
       </c>
       <c r="U13" t="n">
-        <v>1178</v>
+        <v>1187</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0621</v>
+        <v>0.0617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-11
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-02" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-03" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-02)</t>
+          <t>October (through 10-03)</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1313,22 +1313,22 @@
         <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="U12" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -1359,46 +1359,46 @@
         <v>52</v>
       </c>
       <c r="I13" t="n">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0819</v>
+        <v>0.08160000000000001</v>
       </c>
       <c r="K13" t="n">
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1103</v>
+        <v>0.1097</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1017</v>
+        <v>0.1014</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0582</v>
+        <v>0.058</v>
       </c>
       <c r="T13" t="n">
         <v>78</v>
       </c>
       <c r="U13" t="n">
-        <v>1187</v>
+        <v>1200</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0617</v>
+        <v>0.061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-12
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-03" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-04" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1288,23 +1288,23 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U11" t="n">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0112</v>
+        <v>0.0169</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-03)</t>
+          <t>October (through 10-04)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>6</v>
@@ -1319,16 +1319,16 @@
         <v>0.2</v>
       </c>
       <c r="L12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="U12" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
@@ -1341,10 +1341,10 @@
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.131</v>
+        <v>0.1304</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
@@ -1368,37 +1368,37 @@
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1097</v>
+        <v>0.1093</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1014</v>
+        <v>0.1012</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>861</v>
+        <v>870</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.058</v>
+        <v>0.0574</v>
       </c>
       <c r="T13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="U13" t="n">
         <v>1200</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.061</v>
+        <v>0.0618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-13
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-05" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -737,10 +737,10 @@
         <v>15</v>
       </c>
       <c r="U3" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0.0694</v>
+        <v>0.06909999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1300,35 +1300,41 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-04)</t>
-        </is>
+          <t>October (through 10-05)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>4</v>
       </c>
+      <c r="D12" s="1" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1818</v>
       </c>
       <c r="L12" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="U12" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -1338,67 +1344,67 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" t="n">
         <v>200</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.1342</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1057</v>
+        <v>0.1055</v>
       </c>
       <c r="H13" t="n">
         <v>52</v>
       </c>
       <c r="I13" t="n">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08160000000000001</v>
+        <v>0.0815</v>
       </c>
       <c r="K13" t="n">
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1093</v>
+        <v>0.1089</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1012</v>
+        <v>0.1009</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0574</v>
+        <v>0.057</v>
       </c>
       <c r="T13" t="n">
         <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1200</v>
+        <v>1205</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0618</v>
+        <v>0.0615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-14
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-05" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-06" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,20 +1300,20 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-05)</t>
+          <t>October (through 10-06)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1667</v>
       </c>
       <c r="F12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
@@ -1325,16 +1325,16 @@
         <v>0.1818</v>
       </c>
       <c r="L12" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R12" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="U12" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -1347,19 +1347,19 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1342</v>
+        <v>0.1336</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1055</v>
+        <v>0.105</v>
       </c>
       <c r="H13" t="n">
         <v>52</v>
@@ -1374,37 +1374,37 @@
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1089</v>
+        <v>0.1083</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1009</v>
+        <v>0.1002</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.057</v>
+        <v>0.0567</v>
       </c>
       <c r="T13" t="n">
         <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1205</v>
+        <v>1216</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0615</v>
+        <v>0.061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-15
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-06" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-07" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1288,19 +1288,19 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U11" t="n">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0169</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-06)</t>
+          <t>October (through 10-07)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1313,7 +1313,7 @@
         <v>0.1667</v>
       </c>
       <c r="F12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
@@ -1325,16 +1325,16 @@
         <v>0.1818</v>
       </c>
       <c r="L12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O12" t="n">
         <v>7</v>
       </c>
       <c r="R12" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U12" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -1356,10 +1356,10 @@
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.105</v>
+        <v>0.1048</v>
       </c>
       <c r="H13" t="n">
         <v>52</v>
@@ -1374,10 +1374,10 @@
         <v>61</v>
       </c>
       <c r="L13" t="n">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1083</v>
+        <v>0.1082</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
@@ -1392,19 +1392,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0567</v>
+        <v>0.0566</v>
       </c>
       <c r="T13" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U13" t="n">
-        <v>1216</v>
+        <v>1220</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.061</v>
+        <v>0.0615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-16
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-07" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-08" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1078,13 +1078,13 @@
         <v>0.0789</v>
       </c>
       <c r="T8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U8" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="V8" s="1" t="n">
-        <v>0.0308</v>
+        <v>0.0231</v>
       </c>
     </row>
     <row r="9">
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-07)</t>
+          <t>October (through 10-08)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1313,28 +1313,34 @@
         <v>0.1667</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1818</v>
+        <v>0.1667</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>0.0526</v>
       </c>
       <c r="O12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R12" t="n">
         <v>35</v>
       </c>
       <c r="U12" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -1356,37 +1362,37 @@
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1036</v>
       </c>
       <c r="H13" t="n">
         <v>52</v>
       </c>
       <c r="I13" t="n">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0815</v>
+        <v>0.0814</v>
       </c>
       <c r="K13" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L13" t="n">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1082</v>
+        <v>0.1093</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1002</v>
+        <v>0.1</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
@@ -1398,13 +1404,13 @@
         <v>0.0566</v>
       </c>
       <c r="T13" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1220</v>
+        <v>1226</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0615</v>
+        <v>0.0605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-17
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-08" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-09" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1291,56 +1291,56 @@
         <v>4</v>
       </c>
       <c r="U11" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0225</v>
+        <v>0.0223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-08)</t>
+          <t>October (through 10-09)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.1429</v>
       </c>
       <c r="F12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" t="n">
+        <v>4</v>
+      </c>
+      <c r="I12" t="n">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>0.2353</v>
+      </c>
+      <c r="K12" t="n">
         <v>2</v>
       </c>
-      <c r="I12" t="n">
-        <v>10</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>0.1667</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
       <c r="L12" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="O12" t="n">
         <v>8</v>
       </c>
       <c r="R12" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="U12" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -1353,37 +1353,37 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1336</v>
+        <v>0.133</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1036</v>
+        <v>0.1034</v>
       </c>
       <c r="H13" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I13" t="n">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0814</v>
+        <v>0.0839</v>
       </c>
       <c r="K13" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1093</v>
+        <v>0.1103</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
@@ -1398,19 +1398,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0566</v>
+        <v>0.0564</v>
       </c>
       <c r="T13" t="n">
         <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1226</v>
+        <v>1231</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0605</v>
+        <v>0.0603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-18
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-09" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-10" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,20 +1300,20 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-09)</t>
+          <t>October (through 10-10)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.125</v>
       </c>
       <c r="F12" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
@@ -1328,19 +1328,19 @@
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="O12" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="R12" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="U12" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -1353,19 +1353,19 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.133</v>
+        <v>0.1325</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1031</v>
       </c>
       <c r="H13" t="n">
         <v>54</v>
@@ -1380,37 +1380,37 @@
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1103</v>
+        <v>0.1099</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
       </c>
       <c r="O13" t="n">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0993</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>886</v>
+        <v>891</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0564</v>
+        <v>0.0561</v>
       </c>
       <c r="T13" t="n">
         <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1231</v>
+        <v>1237</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0603</v>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-19
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-11" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,47 +1300,47 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-10)</t>
+          <t>October (through 10-11)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
       </c>
       <c r="I12" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2353</v>
+        <v>0.2222</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.08</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="O12" t="n">
         <v>11</v>
       </c>
       <c r="R12" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="U12" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -1353,37 +1353,37 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1325</v>
+        <v>0.1314</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
       </c>
       <c r="F13" t="n">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1029</v>
       </c>
       <c r="H13" t="n">
         <v>54</v>
       </c>
       <c r="I13" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0839</v>
+        <v>0.0837</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1099</v>
+        <v>0.1092</v>
       </c>
       <c r="N13" t="n">
         <v>43</v>
@@ -1398,19 +1398,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>891</v>
+        <v>898</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0561</v>
+        <v>0.0557</v>
       </c>
       <c r="T13" t="n">
         <v>79</v>
       </c>
       <c r="U13" t="n">
-        <v>1237</v>
+        <v>1243</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.06</v>
+        <v>0.0598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-20
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-11" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1218,13 +1218,13 @@
         <v>0.0491</v>
       </c>
       <c r="T10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U10" t="n">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.044</v>
+        <v>0.0503</v>
       </c>
     </row>
     <row r="11">
@@ -1300,17 +1300,17 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-11)</t>
+          <t>October (through 10-12)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0833</v>
       </c>
       <c r="F12" t="n">
         <v>18</v>
@@ -1319,28 +1319,34 @@
         <v>4</v>
       </c>
       <c r="I12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2222</v>
+        <v>0.2105</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.0667</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>0.07140000000000001</v>
       </c>
       <c r="R12" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="U12" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
@@ -1353,10 +1359,10 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1314</v>
+        <v>0.1303</v>
       </c>
       <c r="E13" t="n">
         <v>46</v>
@@ -1371,46 +1377,46 @@
         <v>54</v>
       </c>
       <c r="I13" t="n">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0837</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1092</v>
+        <v>0.109</v>
       </c>
       <c r="N13" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O13" t="n">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0993</v>
+        <v>0.1009</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0557</v>
+        <v>0.0554</v>
       </c>
       <c r="T13" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U13" t="n">
-        <v>1243</v>
+        <v>1249</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0598</v>
+        <v>0.0602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-21
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-13" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1148,13 +1148,13 @@
         <v>0.0201</v>
       </c>
       <c r="T9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="U9" t="n">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.0728</v>
+        <v>0.0795</v>
       </c>
     </row>
     <row r="10">
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-12)</t>
+          <t>October (through 10-13)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1312,41 +1312,47 @@
       <c r="D12" s="1" t="n">
         <v>0.0833</v>
       </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
       <c r="F12" t="n">
         <v>18</v>
       </c>
+      <c r="G12" s="1" t="n">
+        <v>0.0526</v>
+      </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2105</v>
+        <v>0.2381</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.0625</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0588</v>
       </c>
       <c r="R12" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="U12" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
@@ -1365,58 +1371,58 @@
         <v>0.1303</v>
       </c>
       <c r="E13" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F13" t="n">
         <v>401</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1029</v>
+        <v>0.1049</v>
       </c>
       <c r="H13" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I13" t="n">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08359999999999999</v>
+        <v>0.0849</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.109</v>
+        <v>0.1086</v>
       </c>
       <c r="N13" t="n">
         <v>44</v>
       </c>
       <c r="O13" t="n">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1009</v>
+        <v>0.1002</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0554</v>
+        <v>0.055</v>
       </c>
       <c r="T13" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U13" t="n">
         <v>1249</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0602</v>
+        <v>0.0609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-22
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-14" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -938,13 +938,13 @@
         <v>0.0625</v>
       </c>
       <c r="T6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U6" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="7">
@@ -1300,59 +1300,59 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-13)</t>
+          <t>October (through 10-14)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.0769</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="H12" t="n">
         <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2381</v>
+        <v>0.2174</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.0556</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0526</v>
       </c>
       <c r="R12" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U12" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13">
@@ -1365,64 +1365,64 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1303</v>
+        <v>0.1297</v>
       </c>
       <c r="E13" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F13" t="n">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1049</v>
+        <v>0.1064</v>
       </c>
       <c r="H13" t="n">
         <v>55</v>
       </c>
       <c r="I13" t="n">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0849</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1086</v>
+        <v>0.1079</v>
       </c>
       <c r="N13" t="n">
         <v>44</v>
       </c>
       <c r="O13" t="n">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1002</v>
+        <v>0.0998</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.055</v>
+        <v>0.0549</v>
       </c>
       <c r="T13" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1249</v>
+        <v>1254</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0609</v>
+        <v>0.0614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-23
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-14" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-15" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-14)</t>
+          <t>October (through 10-15)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1313,31 +1313,31 @@
         <v>0.0769</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.1154</v>
       </c>
       <c r="H12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I12" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2174</v>
+        <v>0.2069</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0556</v>
+        <v>0.0526</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
@@ -1349,10 +1349,10 @@
         <v>0.0526</v>
       </c>
       <c r="R12" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="U12" t="n">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
@@ -1371,31 +1371,31 @@
         <v>0.1297</v>
       </c>
       <c r="E13" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1064</v>
+        <v>0.1077</v>
       </c>
       <c r="H13" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I13" t="n">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.0854</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1079</v>
+        <v>0.1075</v>
       </c>
       <c r="N13" t="n">
         <v>44</v>
@@ -1410,19 +1410,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>913</v>
+        <v>923</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0549</v>
+        <v>0.0543</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1254</v>
+        <v>1263</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0614</v>
+        <v>0.061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-24
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-16" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-15)</t>
+          <t>October (through 10-16)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1316,43 +1316,43 @@
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1154</v>
+        <v>0.1034</v>
       </c>
       <c r="H12" t="n">
         <v>6</v>
       </c>
       <c r="I12" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2069</v>
+        <v>0.2</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.0488</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.05</v>
       </c>
       <c r="R12" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="U12" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -1374,55 +1374,55 @@
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1077</v>
+        <v>0.107</v>
       </c>
       <c r="H13" t="n">
         <v>56</v>
       </c>
       <c r="I13" t="n">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0854</v>
+        <v>0.0852</v>
       </c>
       <c r="K13" t="n">
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1075</v>
+        <v>0.107</v>
       </c>
       <c r="N13" t="n">
         <v>44</v>
       </c>
       <c r="O13" t="n">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0998</v>
+        <v>0.09950000000000001</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0543</v>
+        <v>0.054</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.061</v>
+        <v>0.0608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-25
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-16" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-17" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1288,29 +1288,29 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U11" t="n">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0223</v>
+        <v>0.0281</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-16)</t>
+          <t>October (through 10-17)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
@@ -1334,10 +1334,10 @@
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0488</v>
+        <v>0.0444</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
@@ -1349,10 +1349,10 @@
         <v>0.05</v>
       </c>
       <c r="R12" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="U12" t="n">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
@@ -1365,10 +1365,10 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1297</v>
+        <v>0.1292</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
@@ -1392,10 +1392,10 @@
         <v>63</v>
       </c>
       <c r="L13" t="n">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.107</v>
+        <v>0.1062</v>
       </c>
       <c r="N13" t="n">
         <v>44</v>
@@ -1410,19 +1410,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.054</v>
+        <v>0.0539</v>
       </c>
       <c r="T13" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="U13" t="n">
-        <v>1266</v>
+        <v>1271</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0608</v>
+        <v>0.0613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-26
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-17" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-18" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1151,10 +1151,10 @@
         <v>12</v>
       </c>
       <c r="U9" t="n">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.0795</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="10">
@@ -1300,17 +1300,17 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-17)</t>
+          <t>October (through 10-18)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0588</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
@@ -1322,37 +1322,37 @@
         <v>0.1034</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I12" t="n">
         <v>24</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2</v>
+        <v>0.2258</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12" t="n">
         <v>43</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0444</v>
+        <v>0.06519999999999999</v>
       </c>
       <c r="N12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.05</v>
+        <v>0.1071</v>
       </c>
       <c r="R12" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="U12" t="n">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
@@ -1365,10 +1365,10 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1292</v>
+        <v>0.1276</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
@@ -1380,49 +1380,49 @@
         <v>0.107</v>
       </c>
       <c r="H13" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I13" t="n">
         <v>601</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0852</v>
+        <v>0.0866</v>
       </c>
       <c r="K13" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L13" t="n">
         <v>530</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1062</v>
+        <v>0.1077</v>
       </c>
       <c r="N13" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O13" t="n">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.09950000000000001</v>
+        <v>0.1022</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0539</v>
+        <v>0.0537</v>
       </c>
       <c r="T13" t="n">
         <v>83</v>
       </c>
       <c r="U13" t="n">
-        <v>1271</v>
+        <v>1277</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0613</v>
+        <v>0.061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-27
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-18" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-19" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,44 +1300,44 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-18)</t>
+          <t>October (through 10-19)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0556</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2258</v>
+        <v>0.2188</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.06519999999999999</v>
+        <v>0.0638</v>
       </c>
       <c r="N12" t="n">
         <v>3</v>
@@ -1349,10 +1349,10 @@
         <v>0.1071</v>
       </c>
       <c r="R12" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="U12" t="n">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
@@ -1365,37 +1365,37 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1276</v>
+        <v>0.127</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.107</v>
+        <v>0.1068</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0866</v>
+        <v>0.08649999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1077</v>
+        <v>0.1076</v>
       </c>
       <c r="N13" t="n">
         <v>46</v>
@@ -1410,19 +1410,19 @@
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0537</v>
+        <v>0.0535</v>
       </c>
       <c r="T13" t="n">
         <v>83</v>
       </c>
       <c r="U13" t="n">
-        <v>1277</v>
+        <v>1289</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.061</v>
+        <v>0.0605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-28
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-19" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-20" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1151,10 +1151,10 @@
         <v>12</v>
       </c>
       <c r="U9" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0805</v>
       </c>
     </row>
     <row r="10">
@@ -1300,59 +1300,59 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-19)</t>
+          <t>October (through 10-20)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>17</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0556</v>
+        <v>0.1053</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09379999999999999</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2188</v>
+        <v>0.2</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0638</v>
+        <v>0.0625</v>
       </c>
       <c r="N12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.129</v>
       </c>
       <c r="R12" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="U12" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13">
@@ -1362,67 +1362,67 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="n">
         <v>213</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.127</v>
+        <v>0.1306</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1068</v>
+        <v>0.1063</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08649999999999999</v>
+        <v>0.0861</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1076</v>
+        <v>0.1074</v>
       </c>
       <c r="N13" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1022</v>
+        <v>0.1038</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0535</v>
+        <v>0.0533</v>
       </c>
       <c r="T13" t="n">
         <v>83</v>
       </c>
       <c r="U13" t="n">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0605</v>
+        <v>0.0604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-29
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-21" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1148,13 +1148,13 @@
         <v>0.0201</v>
       </c>
       <c r="T9" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U9" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.0805</v>
+        <v>0.0738</v>
       </c>
     </row>
     <row r="10">
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-20)</t>
+          <t>October (through 10-21)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1316,43 +1316,43 @@
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.09379999999999999</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1667</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.06</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.129</v>
+        <v>0.1176</v>
       </c>
       <c r="R12" t="n">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="U12" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
@@ -1374,55 +1374,55 @@
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1063</v>
+        <v>0.1061</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>605</v>
+        <v>612</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0861</v>
+        <v>0.0852</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1074</v>
+        <v>0.107</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1038</v>
+        <v>0.1031</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>941</v>
+        <v>949</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0533</v>
+        <v>0.0529</v>
       </c>
       <c r="T13" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1291</v>
+        <v>1294</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0604</v>
+        <v>0.0596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-30
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-22" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-21)</t>
+          <t>October (through 10-22)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1316,43 +1316,43 @@
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.1489</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.06</v>
+        <v>0.0588</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1111</v>
       </c>
       <c r="R12" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="U12" t="n">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13">
@@ -1374,55 +1374,55 @@
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1061</v>
+        <v>0.1052</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0852</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.107</v>
+        <v>0.1068</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1026</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0529</v>
+        <v>0.0528</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1294</v>
+        <v>1300</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0596</v>
+        <v>0.0593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-10-31
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-23" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,59 +1300,59 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-22)</t>
+          <t>October (through 10-23)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.08110000000000001</v>
+        <v>0.0769</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1489</v>
+        <v>0.14</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0577</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1026</v>
       </c>
       <c r="R12" t="n">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="U12" t="n">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13">
@@ -1365,64 +1365,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1306</v>
+        <v>0.1301</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1052</v>
+        <v>0.1047</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.0842</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1068</v>
+        <v>0.1067</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1026</v>
+        <v>0.102</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>951</v>
+        <v>959</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0528</v>
+        <v>0.0524</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1300</v>
+        <v>1312</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0593</v>
+        <v>0.0588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-01
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-23" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-24" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,35 +1300,35 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-23)</t>
+          <t>October (through 10-24)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.075</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
       </c>
       <c r="I12" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.14</v>
+        <v>0.1296</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
@@ -1343,16 +1343,16 @@
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.1026</v>
+        <v>0.09760000000000001</v>
       </c>
       <c r="R12" t="n">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="U12" t="n">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13">
@@ -1365,28 +1365,28 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1301</v>
+        <v>0.1296</v>
       </c>
       <c r="E13" t="n">
         <v>49</v>
       </c>
       <c r="F13" t="n">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1047</v>
+        <v>0.1045</v>
       </c>
       <c r="H13" t="n">
         <v>57</v>
       </c>
       <c r="I13" t="n">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0842</v>
+        <v>0.0837</v>
       </c>
       <c r="K13" t="n">
         <v>64</v>
@@ -1401,28 +1401,28 @@
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.102</v>
+        <v>0.1015</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0524</v>
+        <v>0.0519</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1312</v>
+        <v>1317</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-02
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-25" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,59 +1300,59 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-24)</t>
+          <t>October (through 10-25)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>37</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.075</v>
+        <v>0.09760000000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I12" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1296</v>
+        <v>0.1379</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0577</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.09760000000000001</v>
+        <v>0.093</v>
       </c>
       <c r="R12" t="n">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="U12" t="n">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13">
@@ -1365,64 +1365,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1296</v>
+        <v>0.1285</v>
       </c>
       <c r="E13" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F13" t="n">
         <v>420</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1045</v>
+        <v>0.1064</v>
       </c>
       <c r="H13" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I13" t="n">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0837</v>
+        <v>0.0847</v>
       </c>
       <c r="K13" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L13" t="n">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1067</v>
+        <v>0.1095</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1015</v>
+        <v>0.1011</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>968</v>
+        <v>973</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0519</v>
+        <v>0.0517</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1317</v>
+        <v>1324</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0586</v>
+        <v>0.0583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-03
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-25" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-26" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,59 +1300,59 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-25)</t>
+          <t>October (through 10-26)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.09760000000000001</v>
+        <v>0.1136</v>
       </c>
       <c r="H12" t="n">
         <v>8</v>
       </c>
       <c r="I12" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1379</v>
+        <v>0.1356</v>
       </c>
       <c r="K12" t="n">
         <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.0893</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.093</v>
+        <v>0.0851</v>
       </c>
       <c r="R12" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U12" t="n">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
@@ -1365,64 +1365,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1285</v>
+        <v>0.1275</v>
       </c>
       <c r="E13" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" t="n">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1064</v>
+        <v>0.1078</v>
       </c>
       <c r="H13" t="n">
         <v>58</v>
       </c>
       <c r="I13" t="n">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0847</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="K13" t="n">
         <v>66</v>
       </c>
       <c r="L13" t="n">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1095</v>
+        <v>0.1093</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1011</v>
+        <v>0.1002</v>
       </c>
       <c r="Q13" t="n">
         <v>53</v>
       </c>
       <c r="R13" t="n">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0517</v>
+        <v>0.0516</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1324</v>
+        <v>1330</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0583</v>
+        <v>0.0581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-04
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-26" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-27" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,17 +1300,17 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-26)</t>
+          <t>October (through 10-27)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0741</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
@@ -1325,34 +1325,40 @@
         <v>8</v>
       </c>
       <c r="I12" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1356</v>
+        <v>0.1194</v>
       </c>
       <c r="K12" t="n">
         <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0893</v>
+        <v>0.0877</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0851</v>
+        <v>0.0769</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>126</v>
+        <v>132</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>0.0075</v>
       </c>
       <c r="U12" t="n">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13">
@@ -1365,10 +1371,10 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1275</v>
+        <v>0.1265</v>
       </c>
       <c r="E13" t="n">
         <v>51</v>
@@ -1383,46 +1389,46 @@
         <v>58</v>
       </c>
       <c r="I13" t="n">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08450000000000001</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>66</v>
       </c>
       <c r="L13" t="n">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1093</v>
+        <v>0.1091</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1002</v>
+        <v>0.0992</v>
       </c>
       <c r="Q13" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R13" t="n">
-        <v>974</v>
+        <v>980</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0516</v>
+        <v>0.0522</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1330</v>
+        <v>1338</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0581</v>
+        <v>0.0577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-05
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-27" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-28" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,65 +1300,65 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-27)</t>
+          <t>October (through 10-28)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0741</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
       </c>
       <c r="F12" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1136</v>
+        <v>0.1064</v>
       </c>
       <c r="H12" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1194</v>
+        <v>0.1467</v>
       </c>
       <c r="K12" t="n">
         <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.0847</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="Q12" t="n">
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0075</v>
+        <v>0.0074</v>
       </c>
       <c r="U12" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13">
@@ -1371,61 +1371,61 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1265</v>
+        <v>0.126</v>
       </c>
       <c r="E13" t="n">
         <v>51</v>
       </c>
       <c r="F13" t="n">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1078</v>
+        <v>0.1071</v>
       </c>
       <c r="H13" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I13" t="n">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08359999999999999</v>
+        <v>0.08690000000000001</v>
       </c>
       <c r="K13" t="n">
         <v>66</v>
       </c>
       <c r="L13" t="n">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1091</v>
+        <v>0.1087</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0992</v>
+        <v>0.0983</v>
       </c>
       <c r="Q13" t="n">
         <v>54</v>
       </c>
       <c r="R13" t="n">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0522</v>
+        <v>0.0521</v>
       </c>
       <c r="T13" t="n">
         <v>82</v>
       </c>
       <c r="U13" t="n">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>0.0577</v>

</xml_diff>

<commit_message>
Add data for 2021-11-06
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-28" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-29" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1221,10 +1221,10 @@
         <v>8</v>
       </c>
       <c r="U10" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
@@ -1288,77 +1288,83 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U11" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0281</v>
+        <v>0.0337</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-28)</t>
+          <t>October (through 10-29)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1064</v>
+        <v>0.1132</v>
       </c>
       <c r="H12" t="n">
         <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1467</v>
+        <v>0.141</v>
       </c>
       <c r="K12" t="n">
         <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.0847</v>
+        <v>0.0833</v>
       </c>
       <c r="N12" t="n">
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0702</v>
       </c>
       <c r="Q12" t="n">
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0074</v>
+        <v>0.0072</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1</v>
       </c>
       <c r="U12" t="n">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>0.0055</v>
       </c>
     </row>
     <row r="13">
@@ -1371,64 +1377,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.126</v>
+        <v>0.1255</v>
       </c>
       <c r="E13" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" t="n">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.1079</v>
       </c>
       <c r="H13" t="n">
         <v>61</v>
       </c>
       <c r="I13" t="n">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08690000000000001</v>
+        <v>0.08649999999999999</v>
       </c>
       <c r="K13" t="n">
         <v>66</v>
       </c>
       <c r="L13" t="n">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.1086</v>
       </c>
       <c r="N13" t="n">
         <v>47</v>
       </c>
       <c r="O13" t="n">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0983</v>
+        <v>0.09810000000000001</v>
       </c>
       <c r="Q13" t="n">
         <v>54</v>
       </c>
       <c r="R13" t="n">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0521</v>
+        <v>0.0519</v>
       </c>
       <c r="T13" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U13" t="n">
-        <v>1340</v>
+        <v>1345</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0577</v>
+        <v>0.0588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-07
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-29" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-30" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,71 +1300,71 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-29)</t>
+          <t>October (through 10-30)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.0667</v>
       </c>
       <c r="E12" t="n">
         <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.1071</v>
       </c>
       <c r="H12" t="n">
         <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.141</v>
+        <v>0.1392</v>
       </c>
       <c r="K12" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" t="n">
+        <v>59</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>0.09229999999999999</v>
+      </c>
+      <c r="N12" t="n">
         <v>5</v>
       </c>
-      <c r="L12" t="n">
-        <v>55</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>0.0833</v>
-      </c>
-      <c r="N12" t="n">
-        <v>4</v>
-      </c>
       <c r="O12" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0702</v>
+        <v>0.0847</v>
       </c>
       <c r="Q12" t="n">
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0072</v>
+        <v>0.0068</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12" t="n">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0055</v>
+        <v>0.0106</v>
       </c>
     </row>
     <row r="13">
@@ -1377,64 +1377,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.1255</v>
+        <v>0.125</v>
       </c>
       <c r="E13" t="n">
         <v>52</v>
       </c>
       <c r="F13" t="n">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1079</v>
+        <v>0.1072</v>
       </c>
       <c r="H13" t="n">
         <v>61</v>
       </c>
       <c r="I13" t="n">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.08649999999999999</v>
+        <v>0.0864</v>
       </c>
       <c r="K13" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L13" t="n">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1086</v>
+        <v>0.1093</v>
       </c>
       <c r="N13" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O13" t="n">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.09810000000000001</v>
+        <v>0.0998</v>
       </c>
       <c r="Q13" t="n">
         <v>54</v>
       </c>
       <c r="R13" t="n">
-        <v>986</v>
+        <v>995</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0519</v>
+        <v>0.0515</v>
       </c>
       <c r="T13" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U13" t="n">
-        <v>1345</v>
+        <v>1352</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-08
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-30" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-10-31" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,71 +1300,71 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-30)</t>
+          <t>October (through 10-31)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.0625</v>
       </c>
       <c r="E12" t="n">
         <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.1053</v>
       </c>
       <c r="H12" t="n">
         <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.1392</v>
+        <v>0.1325</v>
       </c>
       <c r="K12" t="n">
         <v>6</v>
       </c>
       <c r="L12" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.09229999999999999</v>
+        <v>0.0896</v>
       </c>
       <c r="N12" t="n">
         <v>5</v>
       </c>
       <c r="O12" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.0847</v>
+        <v>0.0833</v>
       </c>
       <c r="Q12" t="n">
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>0.0068</v>
+        <v>0.0064</v>
       </c>
       <c r="T12" t="n">
         <v>2</v>
       </c>
       <c r="U12" t="n">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0106</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="13">
@@ -1377,64 +1377,64 @@
         <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.125</v>
+        <v>0.124</v>
       </c>
       <c r="E13" t="n">
         <v>52</v>
       </c>
       <c r="F13" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1072</v>
+        <v>0.107</v>
       </c>
       <c r="H13" t="n">
         <v>61</v>
       </c>
       <c r="I13" t="n">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0864</v>
+        <v>0.0859</v>
       </c>
       <c r="K13" t="n">
         <v>67</v>
       </c>
       <c r="L13" t="n">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1093</v>
+        <v>0.1089</v>
       </c>
       <c r="N13" t="n">
         <v>48</v>
       </c>
       <c r="O13" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0998</v>
+        <v>0.09959999999999999</v>
       </c>
       <c r="Q13" t="n">
         <v>54</v>
       </c>
       <c r="R13" t="n">
-        <v>995</v>
+        <v>1003</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0515</v>
+        <v>0.0511</v>
       </c>
       <c r="T13" t="n">
         <v>85</v>
       </c>
       <c r="U13" t="n">
-        <v>1352</v>
+        <v>1359</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0592</v>
+        <v>0.0589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-09
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-10-31" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-01" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23.7109375" customWidth="1" min="1" max="1"/>
+    <col width="24.7109375" customWidth="1" min="1" max="1"/>
     <col width="11.7109375" customWidth="1" min="2" max="2"/>
     <col width="14.7109375" customWidth="1" min="3" max="3"/>
     <col width="11.7109375" customWidth="1" style="1" min="4" max="4"/>
@@ -1300,7 +1300,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>October (through 10-31)</t>
+          <t>October</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1370,71 +1370,105 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
+          <t>November (through 11-01)</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>9</v>
+      </c>
+      <c r="U13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" t="n">
         <v>32</v>
       </c>
-      <c r="C13" t="n">
-        <v>226</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0.124</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="C14" t="n">
+        <v>227</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0.1236</v>
+      </c>
+      <c r="E14" t="n">
         <v>52</v>
       </c>
-      <c r="F13" t="n">
-        <v>434</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0.107</v>
-      </c>
-      <c r="H13" t="n">
+      <c r="F14" t="n">
+        <v>437</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.1063</v>
+      </c>
+      <c r="H14" t="n">
         <v>61</v>
       </c>
-      <c r="I13" t="n">
-        <v>649</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>0.0859</v>
-      </c>
-      <c r="K13" t="n">
-        <v>67</v>
-      </c>
-      <c r="L13" t="n">
-        <v>548</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>0.1089</v>
-      </c>
-      <c r="N13" t="n">
+      <c r="I14" t="n">
+        <v>654</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>0.0853</v>
+      </c>
+      <c r="K14" t="n">
+        <v>68</v>
+      </c>
+      <c r="L14" t="n">
+        <v>551</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>0.1099</v>
+      </c>
+      <c r="N14" t="n">
         <v>48</v>
       </c>
-      <c r="O13" t="n">
-        <v>434</v>
-      </c>
-      <c r="P13" s="1" t="n">
-        <v>0.09959999999999999</v>
-      </c>
-      <c r="Q13" t="n">
+      <c r="O14" t="n">
+        <v>435</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>0.0994</v>
+      </c>
+      <c r="Q14" t="n">
         <v>54</v>
       </c>
-      <c r="R13" t="n">
-        <v>1003</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>0.0511</v>
-      </c>
-      <c r="T13" t="n">
+      <c r="R14" t="n">
+        <v>1012</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>0.0507</v>
+      </c>
+      <c r="T14" t="n">
         <v>85</v>
       </c>
-      <c r="U13" t="n">
-        <v>1359</v>
-      </c>
-      <c r="V13" s="1" t="n">
-        <v>0.0589</v>
+      <c r="U14" t="n">
+        <v>1364</v>
+      </c>
+      <c r="V14" s="1" t="n">
+        <v>0.0587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-10
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-02" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -771,13 +771,13 @@
         <v>0.07140000000000001</v>
       </c>
       <c r="K4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L4" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.098</v>
       </c>
       <c r="N4" t="n">
         <v>3</v>
@@ -1370,35 +1370,41 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-01)</t>
+          <t>November (through 11-02)</t>
         </is>
       </c>
       <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" t="n">
         <v>1</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>0.1429</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>7</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.2222</v>
+      </c>
+      <c r="O13" t="n">
         <v>3</v>
       </c>
-      <c r="I13" t="n">
-        <v>5</v>
-      </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" t="n">
-        <v>3</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="O13" t="n">
-        <v>1</v>
-      </c>
       <c r="R13" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="U13" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1411,64 +1417,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1236</v>
+        <v>0.1231</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1063</v>
+        <v>0.1059</v>
       </c>
       <c r="H14" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0853</v>
+        <v>0.08649999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>68</v>
       </c>
       <c r="L14" t="n">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1099</v>
+        <v>0.109</v>
       </c>
       <c r="N14" t="n">
         <v>48</v>
       </c>
       <c r="O14" t="n">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0994</v>
+        <v>0.099</v>
       </c>
       <c r="Q14" t="n">
         <v>54</v>
       </c>
       <c r="R14" t="n">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0505</v>
       </c>
       <c r="T14" t="n">
         <v>85</v>
       </c>
       <c r="U14" t="n">
-        <v>1364</v>
+        <v>1372</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0587</v>
+        <v>0.0583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-11
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-02" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-03" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,41 +1370,41 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-02)</t>
+          <t>November (through 11-03)</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.1</v>
       </c>
       <c r="K13" t="n">
         <v>2</v>
       </c>
       <c r="L13" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.2222</v>
+        <v>0.1429</v>
       </c>
       <c r="O13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R13" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="U13" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -1426,55 +1426,55 @@
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1059</v>
+        <v>0.1057</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.08649999999999999</v>
+        <v>0.0861</v>
       </c>
       <c r="K14" t="n">
         <v>68</v>
       </c>
       <c r="L14" t="n">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.109</v>
+        <v>0.1081</v>
       </c>
       <c r="N14" t="n">
         <v>48</v>
       </c>
       <c r="O14" t="n">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.099</v>
+        <v>0.0988</v>
       </c>
       <c r="Q14" t="n">
         <v>54</v>
       </c>
       <c r="R14" t="n">
-        <v>1016</v>
+        <v>1024</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0505</v>
+        <v>0.0501</v>
       </c>
       <c r="T14" t="n">
         <v>85</v>
       </c>
       <c r="U14" t="n">
-        <v>1372</v>
+        <v>1377</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0583</v>
+        <v>0.0581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-12
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-03" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-04" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1148,13 +1148,13 @@
         <v>0.0201</v>
       </c>
       <c r="T9" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U9" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.0738</v>
+        <v>0.06710000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -1218,13 +1218,13 @@
         <v>0.0491</v>
       </c>
       <c r="T10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U10" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0438</v>
       </c>
     </row>
     <row r="11">
@@ -1370,41 +1370,41 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-03)</t>
+          <t>November (through 11-04)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0625</v>
       </c>
       <c r="K13" t="n">
         <v>2</v>
       </c>
       <c r="L13" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.125</v>
       </c>
       <c r="O13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R13" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="U13" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
@@ -1417,64 +1417,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1231</v>
+        <v>0.1226</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1057</v>
+        <v>0.1048</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0861</v>
+        <v>0.0854</v>
       </c>
       <c r="K14" t="n">
         <v>68</v>
       </c>
       <c r="L14" t="n">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1081</v>
+        <v>0.1078</v>
       </c>
       <c r="N14" t="n">
         <v>48</v>
       </c>
       <c r="O14" t="n">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0988</v>
+        <v>0.0984</v>
       </c>
       <c r="Q14" t="n">
         <v>54</v>
       </c>
       <c r="R14" t="n">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0501</v>
+        <v>0.0498</v>
       </c>
       <c r="T14" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U14" t="n">
-        <v>1377</v>
+        <v>1385</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0581</v>
+        <v>0.0565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-13
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-05" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,11 +1370,11 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-04)</t>
+          <t>November (through 11-05)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>10</v>
@@ -1383,28 +1383,28 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.05</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L13" t="n">
         <v>14</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.125</v>
+        <v>0.1765</v>
       </c>
       <c r="O13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R13" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="U13" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -1417,10 +1417,10 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1226</v>
+        <v>0.1217</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
@@ -1435,46 +1435,46 @@
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0854</v>
+        <v>0.0849</v>
       </c>
       <c r="K14" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L14" t="n">
         <v>563</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1078</v>
+        <v>0.1092</v>
       </c>
       <c r="N14" t="n">
         <v>48</v>
       </c>
       <c r="O14" t="n">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0984</v>
+        <v>0.0982</v>
       </c>
       <c r="Q14" t="n">
         <v>54</v>
       </c>
       <c r="R14" t="n">
-        <v>1031</v>
+        <v>1039</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.0494</v>
       </c>
       <c r="T14" t="n">
         <v>83</v>
       </c>
       <c r="U14" t="n">
-        <v>1385</v>
+        <v>1392</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0565</v>
+        <v>0.0563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-14
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-05" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-06" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,41 +1370,47 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-05)</t>
+          <t>November (through 11-06)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0476</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" t="n">
         <v>14</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1765</v>
+        <v>0.2222</v>
       </c>
       <c r="O13" t="n">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>0.0233</v>
       </c>
       <c r="U13" t="n">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
@@ -1417,64 +1423,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1217</v>
+        <v>0.1208</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1038</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0849</v>
+        <v>0.0848</v>
       </c>
       <c r="K14" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L14" t="n">
         <v>563</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1092</v>
+        <v>0.1106</v>
       </c>
       <c r="N14" t="n">
         <v>48</v>
       </c>
       <c r="O14" t="n">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0982</v>
+        <v>0.0978</v>
       </c>
       <c r="Q14" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R14" t="n">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0494</v>
+        <v>0.05</v>
       </c>
       <c r="T14" t="n">
         <v>83</v>
       </c>
       <c r="U14" t="n">
-        <v>1392</v>
+        <v>1403</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0563</v>
+        <v>0.0559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-15
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-06" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-07" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1358,35 +1358,35 @@
         <v>0.0064</v>
       </c>
       <c r="T12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U12" t="n">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0102</v>
+        <v>0.0153</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-06)</t>
+          <t>November (through 11-07)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0476</v>
+        <v>0.0417</v>
       </c>
       <c r="K13" t="n">
         <v>4</v>
@@ -1397,20 +1397,32 @@
       <c r="M13" s="1" t="n">
         <v>0.2222</v>
       </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
       <c r="O13" t="n">
         <v>9</v>
       </c>
+      <c r="P13" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="Q13" t="n">
         <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0233</v>
+        <v>0.0222</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>0.0208</v>
       </c>
     </row>
     <row r="14">
@@ -1423,28 +1435,28 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1208</v>
+        <v>0.1203</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1038</v>
+        <v>0.1034</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0848</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="K14" t="n">
         <v>70</v>
@@ -1456,31 +1468,31 @@
         <v>0.1106</v>
       </c>
       <c r="N14" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O14" t="n">
         <v>443</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0978</v>
+        <v>0.09959999999999999</v>
       </c>
       <c r="Q14" t="n">
         <v>55</v>
       </c>
       <c r="R14" t="n">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0499</v>
       </c>
       <c r="T14" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="U14" t="n">
-        <v>1403</v>
+        <v>1407</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0559</v>
+        <v>0.057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-16
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-07" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-08" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,59 +1370,59 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-07)</t>
+          <t>November (through 11-08)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0417</v>
+        <v>0.0345</v>
       </c>
       <c r="K13" t="n">
         <v>4</v>
       </c>
       <c r="L13" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.2222</v>
+        <v>0.2</v>
       </c>
       <c r="N13" t="n">
         <v>1</v>
       </c>
       <c r="O13" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0833</v>
       </c>
       <c r="Q13" t="n">
         <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0222</v>
+        <v>0.02</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0208</v>
+        <v>0.0182</v>
       </c>
     </row>
     <row r="14">
@@ -1435,64 +1435,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1203</v>
+        <v>0.1194</v>
       </c>
       <c r="E14" t="n">
         <v>52</v>
       </c>
       <c r="F14" t="n">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.103</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.08450000000000001</v>
+        <v>0.0839</v>
       </c>
       <c r="K14" t="n">
         <v>70</v>
       </c>
       <c r="L14" t="n">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1106</v>
+        <v>0.1102</v>
       </c>
       <c r="N14" t="n">
         <v>49</v>
       </c>
       <c r="O14" t="n">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.09959999999999999</v>
+        <v>0.0992</v>
       </c>
       <c r="Q14" t="n">
         <v>55</v>
       </c>
       <c r="R14" t="n">
-        <v>1047</v>
+        <v>1052</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0499</v>
+        <v>0.0497</v>
       </c>
       <c r="T14" t="n">
         <v>85</v>
       </c>
       <c r="U14" t="n">
-        <v>1407</v>
+        <v>1414</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.057</v>
+        <v>0.0567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-17
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-08" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-09" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1008,13 +1008,13 @@
         <v>0.0417</v>
       </c>
       <c r="T7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U7" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>0.1296</v>
+        <v>0.1389</v>
       </c>
     </row>
     <row r="8">
@@ -1370,59 +1370,65 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-08)</t>
+          <t>November (through 11-09)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0.0455</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0345</v>
+        <v>0.0312</v>
       </c>
       <c r="K13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.2</v>
+        <v>0.2174</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" t="n">
         <v>11</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.1538</v>
       </c>
       <c r="Q13" t="n">
         <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.02</v>
+        <v>0.0175</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0182</v>
+        <v>0.0156</v>
       </c>
     </row>
     <row r="14">
@@ -1435,64 +1441,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1194</v>
+        <v>0.1185</v>
       </c>
       <c r="E14" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F14" t="n">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.103</v>
+        <v>0.1043</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0839</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="K14" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1102</v>
+        <v>0.1113</v>
       </c>
       <c r="N14" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O14" t="n">
         <v>445</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0992</v>
+        <v>0.101</v>
       </c>
       <c r="Q14" t="n">
         <v>55</v>
       </c>
       <c r="R14" t="n">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0497</v>
+        <v>0.0494</v>
       </c>
       <c r="T14" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="U14" t="n">
-        <v>1414</v>
+        <v>1422</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0567</v>
+        <v>0.057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-18
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-09" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-10" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-09)</t>
+          <t>November (through 11-10)</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1380,55 +1380,49 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0455</v>
+        <v>0.0435</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0312</v>
+        <v>0.027</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.2174</v>
+        <v>0.2</v>
       </c>
       <c r="N13" t="n">
         <v>2</v>
       </c>
       <c r="O13" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1538</v>
+        <v>0.1176</v>
       </c>
       <c r="Q13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0175</v>
-      </c>
-      <c r="T13" t="n">
-        <v>1</v>
+        <v>0.0317</v>
       </c>
       <c r="U13" t="n">
-        <v>63</v>
-      </c>
-      <c r="V13" s="1" t="n">
-        <v>0.0156</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -1450,55 +1444,55 @@
         <v>53</v>
       </c>
       <c r="F14" t="n">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1043</v>
+        <v>0.1041</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.08359999999999999</v>
+        <v>0.083</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1113</v>
+        <v>0.1109</v>
       </c>
       <c r="N14" t="n">
         <v>50</v>
       </c>
       <c r="O14" t="n">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.101</v>
+        <v>0.1002</v>
       </c>
       <c r="Q14" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R14" t="n">
-        <v>1059</v>
+        <v>1064</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0494</v>
+        <v>0.05</v>
       </c>
       <c r="T14" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U14" t="n">
-        <v>1422</v>
+        <v>1427</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.057</v>
+        <v>0.0562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-19
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-11" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -938,13 +938,13 @@
         <v>0.0625</v>
       </c>
       <c r="T6" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="U6" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="7">
@@ -1358,41 +1358,41 @@
         <v>0.0064</v>
       </c>
       <c r="T12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U12" t="n">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0153</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-10)</t>
+          <t>November (through 11-11)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0435</v>
+        <v>0.0385</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.027</v>
+        <v>0.0238</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
@@ -1404,25 +1404,31 @@
         <v>0.2</v>
       </c>
       <c r="N13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O13" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1579</v>
       </c>
       <c r="Q13" t="n">
         <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0317</v>
+        <v>0.0286</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>0.0135</v>
       </c>
     </row>
     <row r="14">
@@ -1435,28 +1441,28 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1185</v>
+        <v>0.1181</v>
       </c>
       <c r="E14" t="n">
         <v>53</v>
       </c>
       <c r="F14" t="n">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1041</v>
+        <v>0.1035</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.083</v>
+        <v>0.0824</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
@@ -1468,31 +1474,31 @@
         <v>0.1109</v>
       </c>
       <c r="N14" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O14" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1002</v>
+        <v>0.1018</v>
       </c>
       <c r="Q14" t="n">
         <v>56</v>
       </c>
       <c r="R14" t="n">
-        <v>1064</v>
+        <v>1071</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0497</v>
       </c>
       <c r="T14" t="n">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1427</v>
+        <v>1429</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0562</v>
+        <v>0.0586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-20
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-11" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1361,74 +1361,74 @@
         <v>4</v>
       </c>
       <c r="U12" t="n">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0204</v>
+        <v>0.0206</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-11)</t>
+          <t>November (through 11-12)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0385</v>
+        <v>0.0357</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0238</v>
+        <v>0.0204</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1923</v>
       </c>
       <c r="N13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1579</v>
+        <v>0.1905</v>
       </c>
       <c r="Q13" t="n">
         <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0286</v>
+        <v>0.026</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0135</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="14">
@@ -1441,64 +1441,64 @@
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1181</v>
+        <v>0.1176</v>
       </c>
       <c r="E14" t="n">
         <v>53</v>
       </c>
       <c r="F14" t="n">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1035</v>
+        <v>0.1031</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>690</v>
+        <v>697</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0824</v>
+        <v>0.08169999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1109</v>
+        <v>0.1108</v>
       </c>
       <c r="N14" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1018</v>
+        <v>0.1034</v>
       </c>
       <c r="Q14" t="n">
         <v>56</v>
       </c>
       <c r="R14" t="n">
-        <v>1071</v>
+        <v>1078</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0497</v>
+        <v>0.0494</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1429</v>
+        <v>1436</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0586</v>
+        <v>0.0584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-21
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-13" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,65 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-12)</t>
-        </is>
+          <t>November (through 11-13)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>14</v>
       </c>
+      <c r="D13" s="1" t="n">
+        <v>0.0667</v>
+      </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0357</v>
+        <v>0.09379999999999999</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0204</v>
+        <v>0.0169</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1923</v>
+        <v>0.1786</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1905</v>
+        <v>0.1818</v>
       </c>
       <c r="Q13" t="n">
         <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.026</v>
+        <v>0.0247</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.012</v>
+        <v>0.0115</v>
       </c>
     </row>
     <row r="14">
@@ -1438,67 +1444,67 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1209</v>
       </c>
       <c r="E14" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F14" t="n">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1062</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.08169999999999999</v>
+        <v>0.0806</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1108</v>
+        <v>0.1104</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1032</v>
       </c>
       <c r="Q14" t="n">
         <v>56</v>
       </c>
       <c r="R14" t="n">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0494</v>
+        <v>0.0492</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1436</v>
+        <v>1440</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0584</v>
+        <v>0.0582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-22
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-14" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,71 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-13)</t>
+          <t>November (through 11-14)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.0588</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.09379999999999999</v>
+        <v>0.0857</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0169</v>
+        <v>0.0161</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1786</v>
+        <v>0.1724</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1818</v>
+        <v>0.1739</v>
       </c>
       <c r="Q13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R13" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0247</v>
+        <v>0.0345</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0115</v>
+        <v>0.0103</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1209</v>
+        <v>0.12</v>
       </c>
       <c r="E14" t="n">
         <v>55</v>
       </c>
       <c r="F14" t="n">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1062</v>
+        <v>0.1056</v>
       </c>
       <c r="H14" t="n">
         <v>62</v>
       </c>
       <c r="I14" t="n">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.0803</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1104</v>
+        <v>0.1102</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1032</v>
+        <v>0.103</v>
       </c>
       <c r="Q14" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R14" t="n">
-        <v>1082</v>
+        <v>1087</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0492</v>
+        <v>0.0498</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1440</v>
+        <v>1450</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0582</v>
+        <v>0.0578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-23
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-14" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-15" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-14)</t>
+          <t>November (through 11-15)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1392,49 +1392,49 @@
         <v>0.0857</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0161</v>
+        <v>0.0312</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1724</v>
+        <v>0.1562</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1739</v>
+        <v>0.16</v>
       </c>
       <c r="Q13" t="n">
         <v>3</v>
       </c>
       <c r="R13" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0345</v>
+        <v>0.0341</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0103</v>
+        <v>0.009299999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1462,37 +1462,37 @@
         <v>0.1056</v>
       </c>
       <c r="H14" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0803</v>
+        <v>0.0814</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1102</v>
+        <v>0.1097</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.103</v>
+        <v>0.1026</v>
       </c>
       <c r="Q14" t="n">
         <v>57</v>
       </c>
       <c r="R14" t="n">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="S14" s="1" t="n">
         <v>0.0498</v>
@@ -1501,10 +1501,10 @@
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1450</v>
+        <v>1461</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0578</v>
+        <v>0.0574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-24
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-16" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-15)</t>
+          <t>November (through 11-16)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1386,28 +1386,28 @@
         <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0857</v>
+        <v>0.0769</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0312</v>
+        <v>0.0294</v>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1562</v>
+        <v>0.1471</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
@@ -1422,19 +1422,19 @@
         <v>3</v>
       </c>
       <c r="R13" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0341</v>
+        <v>0.0323</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.008800000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -1456,28 +1456,28 @@
         <v>55</v>
       </c>
       <c r="F14" t="n">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1056</v>
+        <v>0.1048</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0814</v>
+        <v>0.081</v>
       </c>
       <c r="K14" t="n">
         <v>71</v>
       </c>
       <c r="L14" t="n">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1097</v>
+        <v>0.1094</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
@@ -1492,19 +1492,19 @@
         <v>57</v>
       </c>
       <c r="R14" t="n">
-        <v>1088</v>
+        <v>1093</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.0496</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1461</v>
+        <v>1467</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0574</v>
+        <v>0.0572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-25
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-16" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-17" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-16)</t>
+          <t>November (through 11-17)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1386,55 +1386,55 @@
         <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.0732</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0294</v>
+        <v>0.0282</v>
       </c>
       <c r="K13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1471</v>
+        <v>0.1622</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.16</v>
+        <v>0.1481</v>
       </c>
       <c r="Q13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R13" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0323</v>
+        <v>0.04</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.008399999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1456,55 +1456,55 @@
         <v>55</v>
       </c>
       <c r="F14" t="n">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1044</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.081</v>
+        <v>0.08069999999999999</v>
       </c>
       <c r="K14" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L14" t="n">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1094</v>
+        <v>0.1104</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1026</v>
+        <v>0.1022</v>
       </c>
       <c r="Q14" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R14" t="n">
-        <v>1093</v>
+        <v>1099</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0496</v>
+        <v>0.0501</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1467</v>
+        <v>1472</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0572</v>
+        <v>0.057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-26
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-17" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-18" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,17 +1370,17 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-17)</t>
+          <t>November (through 11-18)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0556</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
@@ -1395,46 +1395,46 @@
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0282</v>
+        <v>0.027</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1622</v>
+        <v>0.1538</v>
       </c>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1481</v>
+        <v>0.1429</v>
       </c>
       <c r="Q13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R13" t="n">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.04</v>
+        <v>0.0459</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.008399999999999999</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="14">
@@ -1447,10 +1447,10 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1196</v>
       </c>
       <c r="E14" t="n">
         <v>55</v>
@@ -1465,46 +1465,46 @@
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.08069999999999999</v>
+        <v>0.0804</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
       </c>
       <c r="L14" t="n">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1104</v>
+        <v>0.1101</v>
       </c>
       <c r="N14" t="n">
         <v>52</v>
       </c>
       <c r="O14" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1022</v>
+        <v>0.102</v>
       </c>
       <c r="Q14" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R14" t="n">
-        <v>1099</v>
+        <v>1107</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0501</v>
+        <v>0.0506</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1472</v>
+        <v>1478</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.057</v>
+        <v>0.0568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-27
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-18" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-19" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,35 +1370,35 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-18)</t>
+          <t>November (through 11-19)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0556</v>
+        <v>0.0526</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.0732</v>
+        <v>0.093</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.027</v>
+        <v>0.0256</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
@@ -1410,31 +1410,31 @@
         <v>0.1538</v>
       </c>
       <c r="N13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O13" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.1667</v>
       </c>
       <c r="Q13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" t="n">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0459</v>
+        <v>0.0513</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.008</v>
+        <v>0.0076</v>
       </c>
     </row>
     <row r="14">
@@ -1447,28 +1447,28 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1196</v>
+        <v>0.1191</v>
       </c>
       <c r="E14" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1044</v>
+        <v>0.1059</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0804</v>
+        <v>0.0799</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
@@ -1480,31 +1480,31 @@
         <v>0.1101</v>
       </c>
       <c r="N14" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O14" t="n">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.102</v>
+        <v>0.1035</v>
       </c>
       <c r="Q14" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R14" t="n">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0506</v>
+        <v>0.0511</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1478</v>
+        <v>1484</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0568</v>
+        <v>0.0566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-28
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-19" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-20" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,44 +1370,44 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-19)</t>
+          <t>November (through 11-20)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.0476</v>
       </c>
       <c r="E13" t="n">
         <v>4</v>
       </c>
       <c r="F13" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.093</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0256</v>
+        <v>0.0244</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1538</v>
+        <v>0.1429</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
@@ -1422,19 +1422,19 @@
         <v>6</v>
       </c>
       <c r="R13" t="n">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0513</v>
+        <v>0.0472</v>
       </c>
       <c r="T13" t="n">
         <v>1</v>
       </c>
       <c r="U13" t="n">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0076</v>
+        <v>0.0073</v>
       </c>
     </row>
     <row r="14">
@@ -1447,37 +1447,37 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1191</v>
+        <v>0.1183</v>
       </c>
       <c r="E14" t="n">
         <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1059</v>
+        <v>0.1053</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0799</v>
+        <v>0.0795</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
       </c>
       <c r="L14" t="n">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1101</v>
+        <v>0.1096</v>
       </c>
       <c r="N14" t="n">
         <v>53</v>
@@ -1492,19 +1492,19 @@
         <v>60</v>
       </c>
       <c r="R14" t="n">
-        <v>1114</v>
+        <v>1124</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0511</v>
+        <v>0.0507</v>
       </c>
       <c r="T14" t="n">
         <v>89</v>
       </c>
       <c r="U14" t="n">
-        <v>1484</v>
+        <v>1490</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0566</v>
+        <v>0.0564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-29
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-21" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1078,13 +1078,13 @@
         <v>0.0789</v>
       </c>
       <c r="T8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U8" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="V8" s="1" t="n">
-        <v>0.0231</v>
+        <v>0.0308</v>
       </c>
     </row>
     <row r="9">
@@ -1288,13 +1288,13 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U11" t="n">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0337</v>
+        <v>0.0393</v>
       </c>
     </row>
     <row r="12">
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-20)</t>
+          <t>November (through 11-21)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1383,22 +1383,22 @@
         <v>0.0476</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0244</v>
+        <v>0.0235</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
@@ -1413,28 +1413,28 @@
         <v>5</v>
       </c>
       <c r="O13" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.1562</v>
       </c>
       <c r="Q13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R13" t="n">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0472</v>
+        <v>0.049</v>
       </c>
       <c r="T13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U13" t="n">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0073</v>
+        <v>0.0134</v>
       </c>
     </row>
     <row r="14">
@@ -1453,22 +1453,22 @@
         <v>0.1183</v>
       </c>
       <c r="E14" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F14" t="n">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1082</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0795</v>
+        <v>0.07920000000000001</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
@@ -1483,28 +1483,28 @@
         <v>53</v>
       </c>
       <c r="O14" t="n">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1035</v>
+        <v>0.1031</v>
       </c>
       <c r="Q14" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R14" t="n">
-        <v>1124</v>
+        <v>1139</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0508</v>
       </c>
       <c r="T14" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="U14" t="n">
-        <v>1490</v>
+        <v>1499</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0564</v>
+        <v>0.0578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-11-30
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-22" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1358,83 +1358,83 @@
         <v>0.0064</v>
       </c>
       <c r="T12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U12" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0206</v>
+        <v>0.0308</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-21)</t>
+          <t>November (through 11-22)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0476</v>
+        <v>0.0455</v>
       </c>
       <c r="E13" t="n">
         <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1132</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0235</v>
+        <v>0.0227</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.1395</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
       </c>
       <c r="O13" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1562</v>
+        <v>0.1389</v>
       </c>
       <c r="Q13" t="n">
         <v>7</v>
       </c>
       <c r="R13" t="n">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.049</v>
+        <v>0.0461</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U13" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0134</v>
+        <v>0.0199</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1183</v>
+        <v>0.1179</v>
       </c>
       <c r="E14" t="n">
         <v>58</v>
       </c>
       <c r="F14" t="n">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1082</v>
+        <v>0.1076</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.07920000000000001</v>
+        <v>0.0789</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
       </c>
       <c r="L14" t="n">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1096</v>
+        <v>0.1094</v>
       </c>
       <c r="N14" t="n">
         <v>53</v>
       </c>
       <c r="O14" t="n">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1023</v>
       </c>
       <c r="Q14" t="n">
         <v>61</v>
       </c>
       <c r="R14" t="n">
-        <v>1139</v>
+        <v>1148</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0508</v>
+        <v>0.0505</v>
       </c>
       <c r="T14" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="U14" t="n">
         <v>1499</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0578</v>
+        <v>0.0596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-01
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-23" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,71 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-22)</t>
+          <t>November (through 11-23)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0455</v>
+        <v>0.0435</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.1228</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0227</v>
+        <v>0.0225</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1395</v>
+        <v>0.1304</v>
       </c>
       <c r="N13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1389</v>
+        <v>0.15</v>
       </c>
       <c r="Q13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R13" t="n">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0461</v>
+        <v>0.0494</v>
       </c>
       <c r="T13" t="n">
         <v>3</v>
       </c>
       <c r="U13" t="n">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0199</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1179</v>
+        <v>0.1174</v>
       </c>
       <c r="E14" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1076</v>
+        <v>0.1087</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0789</v>
+        <v>0.0788</v>
       </c>
       <c r="K14" t="n">
         <v>72</v>
       </c>
       <c r="L14" t="n">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1094</v>
+        <v>0.1089</v>
       </c>
       <c r="N14" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1023</v>
+        <v>0.1034</v>
       </c>
       <c r="Q14" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R14" t="n">
-        <v>1148</v>
+        <v>1157</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0505</v>
+        <v>0.0509</v>
       </c>
       <c r="T14" t="n">
         <v>95</v>
       </c>
       <c r="U14" t="n">
-        <v>1499</v>
+        <v>1506</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0596</v>
+        <v>0.0593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-02
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-23" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-24" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,71 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-23)</t>
+          <t>November (through 11-24)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0435</v>
+        <v>0.0417</v>
       </c>
       <c r="E13" t="n">
         <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1228</v>
+        <v>0.1167</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0225</v>
+        <v>0.022</v>
       </c>
       <c r="K13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L13" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.1458</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.15</v>
+        <v>0.1395</v>
       </c>
       <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="n">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0494</v>
+        <v>0.046</v>
       </c>
       <c r="T13" t="n">
         <v>3</v>
       </c>
       <c r="U13" t="n">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.019</v>
+        <v>0.0182</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1174</v>
+        <v>0.117</v>
       </c>
       <c r="E14" t="n">
         <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.1081</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0788</v>
+        <v>0.07870000000000001</v>
       </c>
       <c r="K14" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L14" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1089</v>
+        <v>0.1101</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1029</v>
       </c>
       <c r="Q14" t="n">
         <v>62</v>
       </c>
       <c r="R14" t="n">
-        <v>1157</v>
+        <v>1169</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0509</v>
+        <v>0.0504</v>
       </c>
       <c r="T14" t="n">
         <v>95</v>
       </c>
       <c r="U14" t="n">
-        <v>1506</v>
+        <v>1513</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0593</v>
+        <v>0.0591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-03
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-25" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1209,13 +1209,13 @@
         <v>0.08890000000000001</v>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R10" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>0.0491</v>
+        <v>0.0429</v>
       </c>
       <c r="T10" t="n">
         <v>7</v>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-24)</t>
+          <t>November (through 11-25)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1386,55 +1386,55 @@
         <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1167</v>
+        <v>0.1129</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.022</v>
+        <v>0.0213</v>
       </c>
       <c r="K13" t="n">
         <v>7</v>
       </c>
       <c r="L13" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1458</v>
+        <v>0.14</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1395</v>
+        <v>0.1333</v>
       </c>
       <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="n">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.046</v>
+        <v>0.0444</v>
       </c>
       <c r="T13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0182</v>
+        <v>0.0234</v>
       </c>
     </row>
     <row r="14">
@@ -1456,55 +1456,55 @@
         <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1081</v>
+        <v>0.1077</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.07870000000000001</v>
+        <v>0.0784</v>
       </c>
       <c r="K14" t="n">
         <v>73</v>
       </c>
       <c r="L14" t="n">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1101</v>
+        <v>0.1098</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1029</v>
+        <v>0.1025</v>
       </c>
       <c r="Q14" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R14" t="n">
-        <v>1169</v>
+        <v>1176</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0504</v>
+        <v>0.0493</v>
       </c>
       <c r="T14" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1513</v>
+        <v>1518</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0591</v>
+        <v>0.0595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-04
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-25" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-26" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,71 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-25)</t>
+          <t>November (through 11-26)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0417</v>
+        <v>0.0357</v>
       </c>
       <c r="E13" t="n">
         <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1129</v>
+        <v>0.1061</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0213</v>
+        <v>0.0204</v>
       </c>
       <c r="K13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L13" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.14</v>
+        <v>0.1379</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1333</v>
+        <v>0.1304</v>
       </c>
       <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0444</v>
+        <v>0.044</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0234</v>
+        <v>0.0226</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.117</v>
+        <v>0.1154</v>
       </c>
       <c r="E14" t="n">
         <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1077</v>
+        <v>0.1069</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0784</v>
+        <v>0.078</v>
       </c>
       <c r="K14" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L14" t="n">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1098</v>
+        <v>0.11</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1025</v>
+        <v>0.1023</v>
       </c>
       <c r="Q14" t="n">
         <v>61</v>
       </c>
       <c r="R14" t="n">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0493</v>
+        <v>0.0492</v>
       </c>
       <c r="T14" t="n">
         <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1518</v>
+        <v>1524</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0595</v>
+        <v>0.0593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-05
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-26" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-27" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,71 +1370,71 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-26)</t>
+          <t>November (through 11-27)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0357</v>
+        <v>0.0345</v>
       </c>
       <c r="E13" t="n">
         <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1061</v>
+        <v>0.1</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0204</v>
+        <v>0.02</v>
       </c>
       <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1379</v>
+        <v>0.1333</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.1277</v>
       </c>
       <c r="Q13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R13" t="n">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.044</v>
+        <v>0.0521</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0226</v>
+        <v>0.0217</v>
       </c>
     </row>
     <row r="14">
@@ -1447,64 +1447,64 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1154</v>
+        <v>0.115</v>
       </c>
       <c r="E14" t="n">
         <v>59</v>
       </c>
       <c r="F14" t="n">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1069</v>
+        <v>0.1061</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.078</v>
+        <v>0.07779999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>74</v>
       </c>
       <c r="L14" t="n">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.11</v>
+        <v>0.1096</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1023</v>
+        <v>0.1021</v>
       </c>
       <c r="Q14" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="R14" t="n">
-        <v>1178</v>
+        <v>1186</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0492</v>
+        <v>0.0504</v>
       </c>
       <c r="T14" t="n">
         <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1524</v>
+        <v>1531</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0593</v>
+        <v>0.059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-06
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-27" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-28" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-27)</t>
+          <t>November (through 11-28)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1383,58 +1383,58 @@
         <v>0.0345</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1</v>
+        <v>0.1096</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.02</v>
+        <v>0.0198</v>
       </c>
       <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.1333</v>
+        <v>0.127</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.1277</v>
+        <v>0.125</v>
       </c>
       <c r="Q13" t="n">
         <v>10</v>
       </c>
       <c r="R13" t="n">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0521</v>
+        <v>0.0503</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0217</v>
+        <v>0.0211</v>
       </c>
     </row>
     <row r="14">
@@ -1453,58 +1453,58 @@
         <v>0.115</v>
       </c>
       <c r="E14" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" t="n">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1061</v>
+        <v>0.1073</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.07779999999999999</v>
+        <v>0.07770000000000001</v>
       </c>
       <c r="K14" t="n">
         <v>74</v>
       </c>
       <c r="L14" t="n">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1096</v>
+        <v>0.1091</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1021</v>
+        <v>0.1019</v>
       </c>
       <c r="Q14" t="n">
         <v>63</v>
       </c>
       <c r="R14" t="n">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0504</v>
+        <v>0.0502</v>
       </c>
       <c r="T14" t="n">
         <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1531</v>
+        <v>1537</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.059</v>
+        <v>0.0588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-07
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-28" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-29" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -999,13 +999,13 @@
         <v>0.1633</v>
       </c>
       <c r="Q7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>0.0417</v>
+        <v>0.0521</v>
       </c>
       <c r="T7" t="n">
         <v>15</v>
@@ -1370,44 +1370,44 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-28)</t>
+          <t>November (through 11-29)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0345</v>
+        <v>0.0312</v>
       </c>
       <c r="E13" t="n">
         <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1096</v>
+        <v>0.1053</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.0198</v>
+        <v>0.019</v>
       </c>
       <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.127</v>
+        <v>0.1194</v>
       </c>
       <c r="N13" t="n">
         <v>6</v>
@@ -1422,19 +1422,19 @@
         <v>10</v>
       </c>
       <c r="R13" t="n">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.0488</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0211</v>
+        <v>0.0208</v>
       </c>
     </row>
     <row r="14">
@@ -1447,37 +1447,37 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.115</v>
+        <v>0.1138</v>
       </c>
       <c r="E14" t="n">
         <v>60</v>
       </c>
       <c r="F14" t="n">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1073</v>
+        <v>0.1068</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.07770000000000001</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>74</v>
       </c>
       <c r="L14" t="n">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1091</v>
+        <v>0.1085</v>
       </c>
       <c r="N14" t="n">
         <v>54</v>
@@ -1489,22 +1489,22 @@
         <v>0.1019</v>
       </c>
       <c r="Q14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R14" t="n">
-        <v>1193</v>
+        <v>1198</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0502</v>
+        <v>0.0507</v>
       </c>
       <c r="T14" t="n">
         <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1537</v>
+        <v>1539</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-08
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-29" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-11-30" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1370,35 +1370,35 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-29)</t>
+          <t>November (through 11-30)</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.0312</v>
+        <v>0.0303</v>
       </c>
       <c r="E13" t="n">
         <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1039</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="K13" t="n">
         <v>8</v>
@@ -1413,28 +1413,28 @@
         <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.125</v>
+        <v>0.1154</v>
       </c>
       <c r="Q13" t="n">
         <v>10</v>
       </c>
       <c r="R13" t="n">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0.0488</v>
+        <v>0.0483</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
       </c>
       <c r="U13" t="n">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0208</v>
+        <v>0.0198</v>
       </c>
     </row>
     <row r="14">
@@ -1447,28 +1447,28 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1138</v>
+        <v>0.1134</v>
       </c>
       <c r="E14" t="n">
         <v>60</v>
       </c>
       <c r="F14" t="n">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1068</v>
+        <v>0.1066</v>
       </c>
       <c r="H14" t="n">
         <v>63</v>
       </c>
       <c r="I14" t="n">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.07729999999999999</v>
+        <v>0.0767</v>
       </c>
       <c r="K14" t="n">
         <v>74</v>
@@ -1483,28 +1483,28 @@
         <v>54</v>
       </c>
       <c r="O14" t="n">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1019</v>
+        <v>0.1011</v>
       </c>
       <c r="Q14" t="n">
         <v>64</v>
       </c>
       <c r="R14" t="n">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0506</v>
       </c>
       <c r="T14" t="n">
         <v>96</v>
       </c>
       <c r="U14" t="n">
-        <v>1539</v>
+        <v>1549</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0587</v>
+        <v>0.0584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-09
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-11-30" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-01" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1291,10 +1291,10 @@
         <v>7</v>
       </c>
       <c r="U11" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0393</v>
+        <v>0.0395</v>
       </c>
     </row>
     <row r="12">
@@ -1370,7 +1370,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>November (through 11-30)</t>
+          <t>November</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1428,83 +1428,105 @@
         <v>0.0483</v>
       </c>
       <c r="T13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0198</v>
+        <v>0.0248</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
+          <t>December (through 12-01)</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+      <c r="L14" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" t="n">
+        <v>4</v>
+      </c>
+      <c r="U14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>33</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>258</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.1134</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>60</v>
       </c>
-      <c r="F14" t="n">
-        <v>503</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>0.1066</v>
-      </c>
-      <c r="H14" t="n">
+      <c r="F15" t="n">
+        <v>506</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="H15" t="n">
         <v>63</v>
       </c>
-      <c r="I14" t="n">
-        <v>758</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0.0767</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="I15" t="n">
+        <v>762</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>0.0764</v>
+      </c>
+      <c r="K15" t="n">
         <v>74</v>
       </c>
-      <c r="L14" t="n">
-        <v>608</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>0.1085</v>
-      </c>
-      <c r="N14" t="n">
+      <c r="L15" t="n">
+        <v>611</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="N15" t="n">
         <v>54</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O15" t="n">
         <v>480</v>
       </c>
-      <c r="P14" s="1" t="n">
+      <c r="P15" s="1" t="n">
         <v>0.1011</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q15" t="n">
         <v>64</v>
       </c>
-      <c r="R14" t="n">
-        <v>1200</v>
-      </c>
-      <c r="S14" s="1" t="n">
-        <v>0.0506</v>
-      </c>
-      <c r="T14" t="n">
-        <v>96</v>
-      </c>
-      <c r="U14" t="n">
-        <v>1549</v>
-      </c>
-      <c r="V14" s="1" t="n">
-        <v>0.0584</v>
+      <c r="R15" t="n">
+        <v>1204</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>0.0505</v>
+      </c>
+      <c r="T15" t="n">
+        <v>97</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1553</v>
+      </c>
+      <c r="V15" s="1" t="n">
+        <v>0.0588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-10
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-02" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,23 +1440,38 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-01)</t>
-        </is>
+          <t>December (through 12-02)</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.1667</v>
       </c>
       <c r="I14" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>0.1429</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U14" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -1475,58 +1490,58 @@
         <v>0.1134</v>
       </c>
       <c r="E15" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.106</v>
+        <v>0.1072</v>
       </c>
       <c r="H15" t="n">
         <v>63</v>
       </c>
       <c r="I15" t="n">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0764</v>
+        <v>0.0762</v>
       </c>
       <c r="K15" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L15" t="n">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.108</v>
+        <v>0.1089</v>
       </c>
       <c r="N15" t="n">
         <v>54</v>
       </c>
       <c r="O15" t="n">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1011</v>
+        <v>0.1007</v>
       </c>
       <c r="Q15" t="n">
         <v>64</v>
       </c>
       <c r="R15" t="n">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0505</v>
+        <v>0.0503</v>
       </c>
       <c r="T15" t="n">
         <v>97</v>
       </c>
       <c r="U15" t="n">
-        <v>1553</v>
+        <v>1561</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0588</v>
+        <v>0.0585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-11
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-02" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-03" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1358,13 +1358,13 @@
         <v>0.0064</v>
       </c>
       <c r="T12" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U12" t="n">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0308</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="13">
@@ -1440,38 +1440,47 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-02)</t>
-        </is>
+          <t>December (through 12-03)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.09089999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.1111</v>
       </c>
       <c r="O14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="U14" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -1481,40 +1490,40 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="n">
         <v>258</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1134</v>
+        <v>0.1164</v>
       </c>
       <c r="E15" t="n">
         <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1072</v>
+        <v>0.1063</v>
       </c>
       <c r="H15" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I15" t="n">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0762</v>
+        <v>0.077</v>
       </c>
       <c r="K15" t="n">
         <v>75</v>
       </c>
       <c r="L15" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1089</v>
+        <v>0.1085</v>
       </c>
       <c r="N15" t="n">
         <v>54</v>
@@ -1529,19 +1538,19 @@
         <v>64</v>
       </c>
       <c r="R15" t="n">
-        <v>1208</v>
+        <v>1213</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.0501</v>
       </c>
       <c r="T15" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1561</v>
+        <v>1565</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0585</v>
+        <v>0.0595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-12
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-03" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-04" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,47 +1440,53 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-03)</t>
+          <t>December (through 12-04)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.0769</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0625</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="U14" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -1493,64 +1499,64 @@
         <v>34</v>
       </c>
       <c r="C15" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1164</v>
+        <v>0.116</v>
       </c>
       <c r="E15" t="n">
         <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1063</v>
+        <v>0.1059</v>
       </c>
       <c r="H15" t="n">
         <v>64</v>
       </c>
       <c r="I15" t="n">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.077</v>
+        <v>0.0765</v>
       </c>
       <c r="K15" t="n">
         <v>75</v>
       </c>
       <c r="L15" t="n">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1085</v>
+        <v>0.1082</v>
       </c>
       <c r="N15" t="n">
         <v>54</v>
       </c>
       <c r="O15" t="n">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1007</v>
+        <v>0.1004</v>
       </c>
       <c r="Q15" t="n">
         <v>64</v>
       </c>
       <c r="R15" t="n">
-        <v>1213</v>
+        <v>1219</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0501</v>
+        <v>0.0499</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1565</v>
+        <v>1576</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0595</v>
+        <v>0.0591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-13
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-05" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1431,44 +1431,44 @@
         <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0248</v>
+        <v>0.0249</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-04)</t>
+          <t>December (through 12-05)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.5</v>
+        <v>0.3333</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.0625</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.1053</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
@@ -1480,13 +1480,19 @@
         <v>0.09089999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>0.0769</v>
       </c>
       <c r="U14" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
@@ -1499,28 +1505,28 @@
         <v>34</v>
       </c>
       <c r="C15" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.116</v>
+        <v>0.1156</v>
       </c>
       <c r="E15" t="n">
         <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1059</v>
+        <v>0.1054</v>
       </c>
       <c r="H15" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I15" t="n">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0765</v>
+        <v>0.0774</v>
       </c>
       <c r="K15" t="n">
         <v>75</v>
@@ -1535,28 +1541,28 @@
         <v>54</v>
       </c>
       <c r="O15" t="n">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1004</v>
+        <v>0.1002</v>
       </c>
       <c r="Q15" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1219</v>
+        <v>1224</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0499</v>
+        <v>0.0512</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1576</v>
+        <v>1581</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0591</v>
+        <v>0.0589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-14
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-05" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-06" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,7 +1440,7 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-05)</t>
+          <t>December (through 12-06)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1456,19 +1456,19 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0625</v>
+        <v>0.0526</v>
       </c>
       <c r="H14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1304</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
@@ -1480,19 +1480,19 @@
         <v>0.09089999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.0645</v>
       </c>
       <c r="U14" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15">
@@ -1514,19 +1514,19 @@
         <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1054</v>
+        <v>0.1048</v>
       </c>
       <c r="H15" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0774</v>
+        <v>0.07820000000000001</v>
       </c>
       <c r="K15" t="n">
         <v>75</v>
@@ -1541,28 +1541,28 @@
         <v>54</v>
       </c>
       <c r="O15" t="n">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1002</v>
+        <v>0.1</v>
       </c>
       <c r="Q15" t="n">
         <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1224</v>
+        <v>1229</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0512</v>
+        <v>0.051</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1581</v>
+        <v>1593</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0589</v>
+        <v>0.0585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-15
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-06" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-07" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1431,23 +1431,23 @@
         <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0249</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-06)</t>
+          <t>December (through 12-07)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0.3333</v>
@@ -1456,43 +1456,49 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0526</v>
+        <v>0.0455</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.12</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.07140000000000001</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>0.125</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0645</v>
+        <v>0.0571</v>
       </c>
       <c r="U14" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
@@ -1502,67 +1508,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1156</v>
+        <v>0.1178</v>
       </c>
       <c r="E15" t="n">
         <v>61</v>
       </c>
       <c r="F15" t="n">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1043</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.07820000000000001</v>
+        <v>0.078</v>
       </c>
       <c r="K15" t="n">
         <v>75</v>
       </c>
       <c r="L15" t="n">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1082</v>
+        <v>0.1078</v>
       </c>
       <c r="N15" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O15" t="n">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1</v>
+        <v>0.1015</v>
       </c>
       <c r="Q15" t="n">
         <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1229</v>
+        <v>1233</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.051</v>
+        <v>0.0508</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1593</v>
+        <v>1600</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0585</v>
+        <v>0.0583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-16
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-07" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-08" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,65 +1440,65 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-07)</t>
+          <t>December (through 12-08)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.3333</v>
+        <v>0.25</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>21</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0455</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.1176</v>
       </c>
       <c r="N14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14" t="n">
         <v>7</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.125</v>
+        <v>0.3</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0571</v>
+        <v>0.0513</v>
       </c>
       <c r="U14" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -1511,64 +1511,64 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1178</v>
+        <v>0.1171</v>
       </c>
       <c r="E15" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F15" t="n">
         <v>524</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1043</v>
+        <v>0.1058</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>780</v>
+        <v>785</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.078</v>
+        <v>0.0776</v>
       </c>
       <c r="K15" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L15" t="n">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1078</v>
+        <v>0.1087</v>
       </c>
       <c r="N15" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O15" t="n">
         <v>487</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1015</v>
+        <v>0.1048</v>
       </c>
       <c r="Q15" t="n">
         <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1233</v>
+        <v>1237</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0508</v>
+        <v>0.0507</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1600</v>
+        <v>1608</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0583</v>
+        <v>0.058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-17
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-08" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-09" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1431,16 +1431,16 @@
         <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.025</v>
+        <v>0.0249</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-08)</t>
+          <t>December (through 12-09)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1456,49 +1456,49 @@
         <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.0769</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0833</v>
       </c>
       <c r="K14" t="n">
         <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.3</v>
+        <v>0.2308</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0513</v>
+        <v>0.0476</v>
       </c>
       <c r="U14" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -1520,55 +1520,55 @@
         <v>62</v>
       </c>
       <c r="F15" t="n">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1058</v>
+        <v>0.1053</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>785</v>
+        <v>791</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0776</v>
+        <v>0.077</v>
       </c>
       <c r="K15" t="n">
         <v>76</v>
       </c>
       <c r="L15" t="n">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.1081</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1042</v>
       </c>
       <c r="Q15" t="n">
         <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1237</v>
+        <v>1240</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0505</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1608</v>
+        <v>1615</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.058</v>
+        <v>0.0578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-18
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-09" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-10" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1361,10 +1361,10 @@
         <v>8</v>
       </c>
       <c r="U12" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.041</v>
+        <v>0.0408</v>
       </c>
     </row>
     <row r="13">
@@ -1440,26 +1440,26 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-09)</t>
+          <t>December (through 12-10)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.25</v>
+        <v>0.2222</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.1071</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
@@ -1474,31 +1474,31 @@
         <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.0833</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.2308</v>
+        <v>0.2143</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0476</v>
+        <v>0.0417</v>
       </c>
       <c r="U14" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -1511,19 +1511,19 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1171</v>
+        <v>0.1167</v>
       </c>
       <c r="E15" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" t="n">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1066</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
@@ -1538,37 +1538,37 @@
         <v>76</v>
       </c>
       <c r="L15" t="n">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1081</v>
+        <v>0.1076</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1042</v>
+        <v>0.104</v>
       </c>
       <c r="Q15" t="n">
         <v>66</v>
       </c>
       <c r="R15" t="n">
-        <v>1240</v>
+        <v>1246</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0505</v>
+        <v>0.0503</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1615</v>
+        <v>1620</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0578</v>
+        <v>0.0576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-19
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-11" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1361,10 +1361,10 @@
         <v>8</v>
       </c>
       <c r="U12" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0408</v>
+        <v>0.0406</v>
       </c>
     </row>
     <row r="13">
@@ -1440,35 +1440,35 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-10)</t>
+          <t>December (through 12-11)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.2222</v>
+        <v>0.2</v>
       </c>
       <c r="E14" t="n">
         <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.1</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.0769</v>
       </c>
       <c r="K14" t="n">
         <v>2</v>
@@ -1483,22 +1483,22 @@
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.2143</v>
+        <v>0.1875</v>
       </c>
       <c r="Q14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0417</v>
+        <v>0.0545</v>
       </c>
       <c r="U14" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -1511,28 +1511,28 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1167</v>
+        <v>0.1163</v>
       </c>
       <c r="E15" t="n">
         <v>63</v>
       </c>
       <c r="F15" t="n">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1066</v>
+        <v>0.1062</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.077</v>
+        <v>0.0767</v>
       </c>
       <c r="K15" t="n">
         <v>76</v>
@@ -1547,28 +1547,28 @@
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.104</v>
+        <v>0.1036</v>
       </c>
       <c r="Q15" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R15" t="n">
-        <v>1246</v>
+        <v>1252</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.0508</v>
       </c>
       <c r="T15" t="n">
         <v>99</v>
       </c>
       <c r="U15" t="n">
-        <v>1620</v>
+        <v>1630</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0576</v>
+        <v>0.0573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-20
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-11" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1218,13 +1218,13 @@
         <v>0.0429</v>
       </c>
       <c r="T10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U10" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0438</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
@@ -1431,74 +1431,74 @@
         <v>5</v>
       </c>
       <c r="U13" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.0249</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-11)</t>
+          <t>December (through 12-12)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1667</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.1176</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.075</v>
       </c>
       <c r="K14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.1111</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1875</v>
+        <v>0.1667</v>
       </c>
       <c r="Q14" t="n">
         <v>3</v>
       </c>
       <c r="R14" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0545</v>
+        <v>0.05</v>
       </c>
       <c r="U14" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -1511,64 +1511,64 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1163</v>
+        <v>0.1155</v>
       </c>
       <c r="E15" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1062</v>
+        <v>0.1072</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>0.0767</v>
       </c>
       <c r="K15" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1076</v>
+        <v>0.1086</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1036</v>
+        <v>0.1033</v>
       </c>
       <c r="Q15" t="n">
         <v>67</v>
       </c>
       <c r="R15" t="n">
-        <v>1252</v>
+        <v>1257</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0508</v>
+        <v>0.0506</v>
       </c>
       <c r="T15" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U15" t="n">
-        <v>1630</v>
+        <v>1634</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0573</v>
+        <v>0.0577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-21
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-13" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1361,10 +1361,10 @@
         <v>8</v>
       </c>
       <c r="U12" t="n">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>0.0406</v>
+        <v>0.0408</v>
       </c>
     </row>
     <row r="13">
@@ -1440,65 +1440,65 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-12)</t>
+          <t>December (through 12-13)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.1538</v>
       </c>
       <c r="E14" t="n">
         <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1053</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.075</v>
+        <v>0.0682</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1071</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1667</v>
+        <v>0.1364</v>
       </c>
       <c r="Q14" t="n">
         <v>3</v>
       </c>
       <c r="R14" t="n">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0455</v>
       </c>
       <c r="U14" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15">
@@ -1511,64 +1511,64 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1155</v>
+        <v>0.1151</v>
       </c>
       <c r="E15" t="n">
         <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1072</v>
+        <v>0.1065</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0767</v>
+        <v>0.07630000000000001</v>
       </c>
       <c r="K15" t="n">
         <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1086</v>
+        <v>0.1085</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1033</v>
+        <v>0.1025</v>
       </c>
       <c r="Q15" t="n">
         <v>67</v>
       </c>
       <c r="R15" t="n">
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0506</v>
+        <v>0.0504</v>
       </c>
       <c r="T15" t="n">
         <v>100</v>
       </c>
       <c r="U15" t="n">
-        <v>1634</v>
+        <v>1638</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0577</v>
+        <v>0.0575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-22
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-14" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,65 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-13)</t>
+          <t>December (through 12-14)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1538</v>
+        <v>0.2</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1136</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0682</v>
+        <v>0.06519999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.0968</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1364</v>
+        <v>0.1304</v>
       </c>
       <c r="Q14" t="n">
         <v>3</v>
       </c>
       <c r="R14" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0455</v>
+        <v>0.0435</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1</v>
       </c>
       <c r="U14" t="n">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="V14" s="1" t="n">
+        <v>0.009900000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -1508,67 +1514,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1151</v>
+        <v>0.1176</v>
       </c>
       <c r="E15" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1065</v>
+        <v>0.1071</v>
       </c>
       <c r="H15" t="n">
         <v>66</v>
       </c>
       <c r="I15" t="n">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.07630000000000001</v>
+        <v>0.0761</v>
       </c>
       <c r="K15" t="n">
         <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1085</v>
+        <v>0.108</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1025</v>
+        <v>0.1023</v>
       </c>
       <c r="Q15" t="n">
         <v>67</v>
       </c>
       <c r="R15" t="n">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0504</v>
+        <v>0.0503</v>
       </c>
       <c r="T15" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="U15" t="n">
-        <v>1638</v>
+        <v>1643</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0575</v>
+        <v>0.0579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-23
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-14" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-15" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1428,83 +1428,83 @@
         <v>0.0483</v>
       </c>
       <c r="T13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U13" t="n">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.025</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-14)</t>
+          <t>December (through 12-15)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1875</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1136</v>
+        <v>0.1087</v>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I14" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.06519999999999999</v>
+        <v>0.09619999999999999</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0968</v>
+        <v>0.0882</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.12</v>
       </c>
       <c r="Q14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0435</v>
+        <v>0.0519</v>
       </c>
       <c r="T14" t="n">
         <v>1</v>
       </c>
       <c r="U14" t="n">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.009900000000000001</v>
+        <v>0.0089</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1173</v>
       </c>
       <c r="E15" t="n">
         <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.1067</v>
       </c>
       <c r="H15" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I15" t="n">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0761</v>
+        <v>0.0779</v>
       </c>
       <c r="K15" t="n">
         <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.108</v>
+        <v>0.1075</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1023</v>
+        <v>0.102</v>
       </c>
       <c r="Q15" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1266</v>
+        <v>1273</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.0507</v>
       </c>
       <c r="T15" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1643</v>
+        <v>1653</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0579</v>
+        <v>0.0581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-24
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-16" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1173,13 +1173,13 @@
         <v>0.0312</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0.0759</v>
+        <v>0.0633</v>
       </c>
       <c r="H10" t="n">
         <v>12</v>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-15)</t>
+          <t>December (through 12-16)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1875</v>
+        <v>0.1579</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.1</v>
       </c>
       <c r="H14" t="n">
         <v>5</v>
       </c>
       <c r="I14" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.09619999999999999</v>
+        <v>0.0877</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0882</v>
+        <v>0.0857</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1111</v>
       </c>
       <c r="Q14" t="n">
         <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0519</v>
+        <v>0.0513</v>
       </c>
       <c r="T14" t="n">
         <v>1</v>
       </c>
       <c r="U14" t="n">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0089</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="15">
@@ -1517,52 +1517,52 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1173</v>
+        <v>0.1161</v>
       </c>
       <c r="E15" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1067</v>
+        <v>0.1044</v>
       </c>
       <c r="H15" t="n">
         <v>68</v>
       </c>
       <c r="I15" t="n">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0779</v>
+        <v>0.0774</v>
       </c>
       <c r="K15" t="n">
         <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1075</v>
+        <v>0.1074</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.102</v>
+        <v>0.1016</v>
       </c>
       <c r="Q15" t="n">
         <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="S15" s="1" t="n">
         <v>0.0507</v>
@@ -1571,10 +1571,10 @@
         <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1653</v>
+        <v>1666</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0581</v>
+        <v>0.0577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-25
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-16" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-17" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,44 +1440,44 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-16)</t>
+          <t>December (through 12-17)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1579</v>
+        <v>0.1429</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.0926</v>
       </c>
       <c r="H14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I14" t="n">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.0896</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0857</v>
+        <v>0.0769</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
@@ -1492,19 +1492,19 @@
         <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0513</v>
+        <v>0.05</v>
       </c>
       <c r="T14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.008</v>
+        <v>0.0157</v>
       </c>
     </row>
     <row r="15">
@@ -1517,37 +1517,37 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1161</v>
+        <v>0.1154</v>
       </c>
       <c r="E15" t="n">
         <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1044</v>
+        <v>0.1037</v>
       </c>
       <c r="H15" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I15" t="n">
-        <v>810</v>
+        <v>819</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0774</v>
+        <v>0.07770000000000001</v>
       </c>
       <c r="K15" t="n">
         <v>77</v>
       </c>
       <c r="L15" t="n">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1074</v>
+        <v>0.1068</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
@@ -1562,19 +1562,19 @@
         <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0506</v>
       </c>
       <c r="T15" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0577</v>
+        <v>0.0582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-26
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-17" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-18" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-17)</t>
+          <t>December (through 12-18)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.1304</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0926</v>
+        <v>0.0877</v>
       </c>
       <c r="H14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I14" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.0896</v>
+        <v>0.1143</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1034</v>
       </c>
       <c r="Q14" t="n">
         <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0482</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0157</v>
+        <v>0.0154</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1154</v>
+        <v>0.1146</v>
       </c>
       <c r="E15" t="n">
         <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1037</v>
+        <v>0.1032</v>
       </c>
       <c r="H15" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I15" t="n">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.07770000000000001</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="K15" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L15" t="n">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1068</v>
+        <v>0.1077</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1016</v>
+        <v>0.1012</v>
       </c>
       <c r="Q15" t="n">
         <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0506</v>
+        <v>0.0505</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1667</v>
+        <v>1670</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0582</v>
+        <v>0.0581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-27
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-18" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-19" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,35 +1440,35 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-18)</t>
+          <t>December (through 12-19)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1304</v>
+        <v>0.125</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.0833</v>
       </c>
       <c r="H14" t="n">
         <v>8</v>
       </c>
       <c r="I14" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1143</v>
+        <v>0.1081</v>
       </c>
       <c r="K14" t="n">
         <v>4</v>
@@ -1483,28 +1483,28 @@
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1</v>
       </c>
       <c r="Q14" t="n">
         <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0482</v>
+        <v>0.0449</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0154</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="15">
@@ -1517,28 +1517,28 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1146</v>
+        <v>0.1143</v>
       </c>
       <c r="E15" t="n">
         <v>64</v>
       </c>
       <c r="F15" t="n">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1032</v>
+        <v>0.1027</v>
       </c>
       <c r="H15" t="n">
         <v>71</v>
       </c>
       <c r="I15" t="n">
-        <v>820</v>
+        <v>824</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.07969999999999999</v>
+        <v>0.0793</v>
       </c>
       <c r="K15" t="n">
         <v>78</v>
@@ -1553,28 +1553,28 @@
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1012</v>
+        <v>0.1011</v>
       </c>
       <c r="Q15" t="n">
         <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1279</v>
+        <v>1285</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0505</v>
+        <v>0.0503</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1670</v>
+        <v>1673</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0581</v>
+        <v>0.058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-28
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-19" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-20" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-19)</t>
+          <t>December (through 12-20)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.125</v>
+        <v>0.1111</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.09379999999999999</v>
       </c>
       <c r="H14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I14" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1081</v>
+        <v>0.1169</v>
       </c>
       <c r="K14" t="n">
         <v>4</v>
       </c>
       <c r="L14" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="Q14" t="n">
         <v>4</v>
       </c>
       <c r="R14" t="n">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0449</v>
+        <v>0.043</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.015</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1143</v>
+        <v>0.1132</v>
       </c>
       <c r="E15" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1027</v>
+        <v>0.1037</v>
       </c>
       <c r="H15" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I15" t="n">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0793</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="K15" t="n">
         <v>78</v>
       </c>
       <c r="L15" t="n">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1077</v>
+        <v>0.1074</v>
       </c>
       <c r="N15" t="n">
         <v>57</v>
       </c>
       <c r="O15" t="n">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1011</v>
+        <v>0.1005</v>
       </c>
       <c r="Q15" t="n">
         <v>68</v>
       </c>
       <c r="R15" t="n">
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0503</v>
+        <v>0.0501</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1673</v>
+        <v>1678</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.058</v>
+        <v>0.0578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-29
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-21" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-20)</t>
+          <t>December (through 12-21)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1071</v>
       </c>
       <c r="E14" t="n">
         <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.09379999999999999</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="H14" t="n">
         <v>9</v>
       </c>
       <c r="I14" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1169</v>
+        <v>0.1111</v>
       </c>
       <c r="K14" t="n">
         <v>4</v>
       </c>
       <c r="L14" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.0851</v>
       </c>
       <c r="N14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.1026</v>
       </c>
       <c r="Q14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R14" t="n">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.043</v>
+        <v>0.051</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0145</v>
+        <v>0.0144</v>
       </c>
     </row>
     <row r="15">
@@ -1517,61 +1517,61 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.1129</v>
       </c>
       <c r="E15" t="n">
         <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1037</v>
+        <v>0.1033</v>
       </c>
       <c r="H15" t="n">
         <v>72</v>
       </c>
       <c r="I15" t="n">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.08019999999999999</v>
+        <v>0.0798</v>
       </c>
       <c r="K15" t="n">
         <v>78</v>
       </c>
       <c r="L15" t="n">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1074</v>
+        <v>0.107</v>
       </c>
       <c r="N15" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1005</v>
+        <v>0.1012</v>
       </c>
       <c r="Q15" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R15" t="n">
-        <v>1289</v>
+        <v>1293</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0501</v>
+        <v>0.0507</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="V15" s="1" t="n">
         <v>0.0578</v>

</xml_diff>

<commit_message>
Add data for 2021-12-30
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-22" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1148,13 +1148,13 @@
         <v>0.0201</v>
       </c>
       <c r="T9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U9" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>0.06710000000000001</v>
+        <v>0.0604</v>
       </c>
     </row>
     <row r="10">
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-21)</t>
+          <t>December (through 12-22)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1071</v>
+        <v>0.1333</v>
       </c>
       <c r="E14" t="n">
         <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="H14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I14" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1136</v>
       </c>
       <c r="K14" t="n">
         <v>4</v>
       </c>
       <c r="L14" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0851</v>
+        <v>0.08</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.1026</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="Q14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R14" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.051</v>
+        <v>0.0577</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0144</v>
+        <v>0.0138</v>
       </c>
     </row>
     <row r="15">
@@ -1514,67 +1514,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1129</v>
+        <v>0.1153</v>
       </c>
       <c r="E15" t="n">
         <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1033</v>
+        <v>0.1028</v>
       </c>
       <c r="H15" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I15" t="n">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0798</v>
+        <v>0.0803</v>
       </c>
       <c r="K15" t="n">
         <v>78</v>
       </c>
       <c r="L15" t="n">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.107</v>
+        <v>0.1066</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1012</v>
+        <v>0.1003</v>
       </c>
       <c r="Q15" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R15" t="n">
-        <v>1293</v>
+        <v>1298</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0507</v>
+        <v>0.0512</v>
       </c>
       <c r="T15" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1679</v>
+        <v>1686</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0578</v>
+        <v>0.057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-12-31
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-23" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-22)</t>
+          <t>December (through 12-23)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1333</v>
+        <v>0.125</v>
       </c>
       <c r="E14" t="n">
         <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.0822</v>
       </c>
       <c r="H14" t="n">
         <v>10</v>
       </c>
       <c r="I14" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1136</v>
+        <v>0.1087</v>
       </c>
       <c r="K14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.08</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.0851</v>
       </c>
       <c r="Q14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R14" t="n">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0577</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0138</v>
+        <v>0.0132</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1153</v>
+        <v>0.1146</v>
       </c>
       <c r="E15" t="n">
         <v>65</v>
       </c>
       <c r="F15" t="n">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1028</v>
+        <v>0.1022</v>
       </c>
       <c r="H15" t="n">
         <v>73</v>
       </c>
       <c r="I15" t="n">
-        <v>836</v>
+        <v>840</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0803</v>
+        <v>0.08</v>
       </c>
       <c r="K15" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1066</v>
+        <v>0.1075</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.1003</v>
+        <v>0.0998</v>
       </c>
       <c r="Q15" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="R15" t="n">
-        <v>1298</v>
+        <v>1304</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0512</v>
+        <v>0.0523</v>
       </c>
       <c r="T15" t="n">
         <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1686</v>
+        <v>1693</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.057</v>
+        <v>0.0568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-01
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-23" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-24" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-23)</t>
+          <t>December (through 12-24)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.125</v>
+        <v>0.1176</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0822</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="H14" t="n">
         <v>10</v>
       </c>
       <c r="I14" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.1064</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.0893</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0851</v>
+        <v>0.08</v>
       </c>
       <c r="Q14" t="n">
         <v>8</v>
       </c>
       <c r="R14" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0132</v>
+        <v>0.0128</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1146</v>
+        <v>0.1138</v>
       </c>
       <c r="E15" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" t="n">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1022</v>
+        <v>0.1031</v>
       </c>
       <c r="H15" t="n">
         <v>73</v>
       </c>
       <c r="I15" t="n">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0798</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1075</v>
+        <v>0.107</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0998</v>
+        <v>0.0993</v>
       </c>
       <c r="Q15" t="n">
         <v>72</v>
       </c>
       <c r="R15" t="n">
-        <v>1304</v>
+        <v>1308</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0523</v>
+        <v>0.0522</v>
       </c>
       <c r="T15" t="n">
         <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1693</v>
+        <v>1697</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0568</v>
+        <v>0.0567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-02
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-25" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-24)</t>
+          <t>December (through 12-25)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1176</v>
+        <v>0.1111</v>
       </c>
       <c r="E14" t="n">
         <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.0854</v>
       </c>
       <c r="H14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I14" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1064</v>
+        <v>0.1134</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0893</v>
+        <v>0.0877</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.08</v>
+        <v>0.0769</v>
       </c>
       <c r="Q14" t="n">
         <v>8</v>
       </c>
       <c r="R14" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.0678</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0128</v>
+        <v>0.0127</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1138</v>
+        <v>0.1131</v>
       </c>
       <c r="E15" t="n">
         <v>66</v>
       </c>
       <c r="F15" t="n">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1023</v>
       </c>
       <c r="H15" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I15" t="n">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0798</v>
+        <v>0.0806</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.107</v>
+        <v>0.1069</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0993</v>
+        <v>0.099</v>
       </c>
       <c r="Q15" t="n">
         <v>72</v>
       </c>
       <c r="R15" t="n">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0522</v>
+        <v>0.0521</v>
       </c>
       <c r="T15" t="n">
         <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0567</v>
+        <v>0.0566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-03
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-25" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-26" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-25)</t>
+          <t>December (through 12-26)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1026</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0854</v>
+        <v>0.0941</v>
       </c>
       <c r="H14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1134</v>
+        <v>0.1188</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.0847</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
       </c>
       <c r="O14" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0769</v>
+        <v>0.0727</v>
       </c>
       <c r="Q14" t="n">
         <v>8</v>
       </c>
       <c r="R14" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0678</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0127</v>
+        <v>0.0124</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1131</v>
+        <v>0.1121</v>
       </c>
       <c r="E15" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1023</v>
+        <v>0.1034</v>
       </c>
       <c r="H15" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I15" t="n">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.0813</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1069</v>
+        <v>0.1066</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
       </c>
       <c r="O15" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.099</v>
+        <v>0.0985</v>
       </c>
       <c r="Q15" t="n">
         <v>72</v>
       </c>
       <c r="R15" t="n">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0521</v>
+        <v>0.052</v>
       </c>
       <c r="T15" t="n">
         <v>102</v>
       </c>
       <c r="U15" t="n">
-        <v>1699</v>
+        <v>1702</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0566</v>
+        <v>0.0565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-04
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-26" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-27" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1218,13 +1218,13 @@
         <v>0.0429</v>
       </c>
       <c r="T10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U10" t="n">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0562</v>
       </c>
     </row>
     <row r="11">
@@ -1440,44 +1440,44 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-26)</t>
+          <t>December (through 12-27)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1026</v>
+        <v>0.1</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0941</v>
+        <v>0.092</v>
       </c>
       <c r="H14" t="n">
         <v>12</v>
       </c>
       <c r="I14" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1188</v>
+        <v>0.1132</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0847</v>
+        <v>0.0781</v>
       </c>
       <c r="N14" t="n">
         <v>4</v>
@@ -1492,19 +1492,19 @@
         <v>8</v>
       </c>
       <c r="R14" t="n">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.06610000000000001</v>
+        <v>0.0635</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0124</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="15">
@@ -1517,37 +1517,37 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1121</v>
+        <v>0.1118</v>
       </c>
       <c r="E15" t="n">
         <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1034</v>
+        <v>0.1031</v>
       </c>
       <c r="H15" t="n">
         <v>75</v>
       </c>
       <c r="I15" t="n">
-        <v>847</v>
+        <v>852</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0813</v>
+        <v>0.0809</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1066</v>
+        <v>0.1059</v>
       </c>
       <c r="N15" t="n">
         <v>58</v>
@@ -1562,19 +1562,19 @@
         <v>72</v>
       </c>
       <c r="R15" t="n">
-        <v>1313</v>
+        <v>1318</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.052</v>
+        <v>0.0518</v>
       </c>
       <c r="T15" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1702</v>
+        <v>1706</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0565</v>
+        <v>0.0569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-05
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-27" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-28" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-27)</t>
+          <t>December (through 12-28)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09520000000000001</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.092</v>
+        <v>0.08790000000000001</v>
       </c>
       <c r="H14" t="n">
         <v>12</v>
       </c>
       <c r="I14" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1132</v>
+        <v>0.1111</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0781</v>
+        <v>0.0735</v>
       </c>
       <c r="N14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0727</v>
+        <v>0.0877</v>
       </c>
       <c r="Q14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R14" t="n">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0635</v>
+        <v>0.0677</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.012</v>
+        <v>0.0118</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1118</v>
+        <v>0.1111</v>
       </c>
       <c r="E15" t="n">
         <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1031</v>
+        <v>0.1024</v>
       </c>
       <c r="H15" t="n">
         <v>75</v>
       </c>
       <c r="I15" t="n">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0809</v>
+        <v>0.08069999999999999</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1059</v>
+        <v>0.1053</v>
       </c>
       <c r="N15" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O15" t="n">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0985</v>
+        <v>0.0998</v>
       </c>
       <c r="Q15" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R15" t="n">
-        <v>1318</v>
+        <v>1324</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0518</v>
+        <v>0.0523</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0569</v>
+        <v>0.0568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-06
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-28" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-29" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-28)</t>
+          <t>December (through 12-29)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.09520000000000001</v>
+        <v>0.09089999999999999</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.08790000000000001</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="H14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I14" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1171</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0735</v>
+        <v>0.0694</v>
       </c>
       <c r="N14" t="n">
         <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0877</v>
+        <v>0.0806</v>
       </c>
       <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0677</v>
+        <v>0.06619999999999999</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0118</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1111</v>
+        <v>0.1104</v>
       </c>
       <c r="E15" t="n">
         <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1024</v>
+        <v>0.1021</v>
       </c>
       <c r="H15" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I15" t="n">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.08069999999999999</v>
+        <v>0.0815</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1053</v>
+        <v>0.1048</v>
       </c>
       <c r="N15" t="n">
         <v>59</v>
       </c>
       <c r="O15" t="n">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0998</v>
+        <v>0.099</v>
       </c>
       <c r="Q15" t="n">
         <v>73</v>
       </c>
       <c r="R15" t="n">
-        <v>1324</v>
+        <v>1327</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0523</v>
+        <v>0.0521</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1710</v>
+        <v>1722</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0568</v>
+        <v>0.0564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-07
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-29" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-30" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1440,71 +1440,71 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-29)</t>
+          <t>December (through 12-30)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.09089999999999999</v>
+        <v>0.1087</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.0833</v>
       </c>
       <c r="H14" t="n">
         <v>13</v>
       </c>
       <c r="I14" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.1171</v>
+        <v>0.114</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0694</v>
+        <v>0.0667</v>
       </c>
       <c r="N14" t="n">
         <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0806</v>
+        <v>0.0781</v>
       </c>
       <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="n">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.06619999999999999</v>
+        <v>0.0621</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.011</v>
+        <v>0.0104</v>
       </c>
     </row>
     <row r="15">
@@ -1514,67 +1514,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="n">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1104</v>
+        <v>0.1128</v>
       </c>
       <c r="E15" t="n">
         <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1021</v>
+        <v>0.1017</v>
       </c>
       <c r="H15" t="n">
         <v>76</v>
       </c>
       <c r="I15" t="n">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0815</v>
+        <v>0.0813</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1048</v>
+        <v>0.1044</v>
       </c>
       <c r="N15" t="n">
         <v>59</v>
       </c>
       <c r="O15" t="n">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.099</v>
+        <v>0.0987</v>
       </c>
       <c r="Q15" t="n">
         <v>73</v>
       </c>
       <c r="R15" t="n">
-        <v>1327</v>
+        <v>1336</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0521</v>
+        <v>0.0518</v>
       </c>
       <c r="T15" t="n">
         <v>103</v>
       </c>
       <c r="U15" t="n">
-        <v>1722</v>
+        <v>1732</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0564</v>
+        <v>0.0561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2022-01-08
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-arrests-by-month-yoy-latest.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-12-30" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Through 2021-12-31" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1209,22 +1209,22 @@
         <v>0.08890000000000001</v>
       </c>
       <c r="Q10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R10" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>0.0429</v>
+        <v>0.0491</v>
       </c>
       <c r="T10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U10" t="n">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>0.0562</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="11">
@@ -1288,13 +1288,13 @@
         <v>0.0427</v>
       </c>
       <c r="T11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U11" t="n">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>0.0395</v>
+        <v>0.0452</v>
       </c>
     </row>
     <row r="12">
@@ -1428,83 +1428,83 @@
         <v>0.0483</v>
       </c>
       <c r="T13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U13" t="n">
         <v>194</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0.03</v>
+        <v>0.0348</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>December (through 12-30)</t>
+          <t>December (through 12-31)</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.1087</v>
+        <v>0.102</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0833</v>
+        <v>0.09</v>
       </c>
       <c r="H14" t="n">
         <v>13</v>
       </c>
       <c r="I14" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0.114</v>
+        <v>0.1121</v>
       </c>
       <c r="K14" t="n">
         <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.061</v>
       </c>
       <c r="N14" t="n">
         <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.0781</v>
+        <v>0.0725</v>
       </c>
       <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.0621</v>
+        <v>0.0604</v>
       </c>
       <c r="T14" t="n">
         <v>2</v>
       </c>
       <c r="U14" t="n">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.0104</v>
+        <v>0.0098</v>
       </c>
     </row>
     <row r="15">
@@ -1517,64 +1517,64 @@
         <v>38</v>
       </c>
       <c r="C15" t="n">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.1128</v>
+        <v>0.1118</v>
       </c>
       <c r="E15" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" t="n">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.1017</v>
+        <v>0.1026</v>
       </c>
       <c r="H15" t="n">
         <v>76</v>
       </c>
       <c r="I15" t="n">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.0813</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="K15" t="n">
         <v>79</v>
       </c>
       <c r="L15" t="n">
-        <v>678</v>
+        <v>685</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.1044</v>
+        <v>0.1034</v>
       </c>
       <c r="N15" t="n">
         <v>59</v>
       </c>
       <c r="O15" t="n">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0987</v>
+        <v>0.0978</v>
       </c>
       <c r="Q15" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R15" t="n">
-        <v>1336</v>
+        <v>1339</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>0.0518</v>
+        <v>0.0524</v>
       </c>
       <c r="T15" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="U15" t="n">
-        <v>1732</v>
+        <v>1742</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.0561</v>
+        <v>0.0574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>